<commit_message>
we create sheet for HomePage and we do several tests on HomePage for logo, right header, footer, ShipTo US and ShipTo internationally and for My Account for US and CAD users and for international users
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,39 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{75299738-06F8-4BE1-91BE-D33B843308C4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" firstSheet="24" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SetupBrowsers" sheetId="50" r:id="rId1"/>
-    <sheet name="SetupRunners" sheetId="51" r:id="rId2"/>
-    <sheet name="USAccountSetupRegression" sheetId="37" r:id="rId3"/>
-    <sheet name="CanadaAccountSetupRegression" sheetId="45" r:id="rId4"/>
-    <sheet name="KioskAccountSetupRegression" sheetId="47" r:id="rId5"/>
-    <sheet name="USCheckOutRegression" sheetId="7" r:id="rId6"/>
-    <sheet name="CSCCheckOutRegression" sheetId="48" r:id="rId7"/>
-    <sheet name="CanadaCheckOutRegression" sheetId="44" r:id="rId8"/>
-    <sheet name="KioskCheckOutRegression" sheetId="46" r:id="rId9"/>
-    <sheet name="CheckOutNegativeCasesRegression" sheetId="53" r:id="rId10"/>
-    <sheet name="EnvoyCheckOutRegression" sheetId="56" r:id="rId11"/>
-    <sheet name="PDPRegression" sheetId="29" r:id="rId12"/>
-    <sheet name="PLPRegression" sheetId="54" r:id="rId13"/>
-    <sheet name="MiniCartRegression" sheetId="57" r:id="rId14"/>
-    <sheet name="CartRegression" sheetId="49" r:id="rId15"/>
-    <sheet name="RegistrationRegression" sheetId="24" r:id="rId16"/>
-    <sheet name="MyAccountRegression" sheetId="27" r:id="rId17"/>
-    <sheet name="LoginRegression" sheetId="41" r:id="rId18"/>
-    <sheet name="CreateAccountsRegression" sheetId="52" r:id="rId19"/>
-    <sheet name="users" sheetId="13" r:id="rId20"/>
-    <sheet name="products" sheetId="55" r:id="rId21"/>
-    <sheet name="cards" sheetId="9" r:id="rId22"/>
-    <sheet name="addresses" sheetId="10" r:id="rId23"/>
-    <sheet name="VisualTestingCLPRegression" sheetId="42" r:id="rId24"/>
-    <sheet name="VisualTestingHPRegression" sheetId="40" r:id="rId25"/>
-    <sheet name="OrderHistoryRegression" sheetId="23" r:id="rId26"/>
-    <sheet name="QuickViewRegression" sheetId="39" r:id="rId27"/>
+    <sheet name="HomePageRegression" sheetId="58" r:id="rId1"/>
+    <sheet name="SetupBrowsers" sheetId="50" r:id="rId2"/>
+    <sheet name="SetupRunners" sheetId="51" r:id="rId3"/>
+    <sheet name="USAccountSetupRegression" sheetId="37" r:id="rId4"/>
+    <sheet name="CanadaAccountSetupRegression" sheetId="45" r:id="rId5"/>
+    <sheet name="KioskAccountSetupRegression" sheetId="47" r:id="rId6"/>
+    <sheet name="USCheckOutRegression" sheetId="7" r:id="rId7"/>
+    <sheet name="CSCCheckOutRegression" sheetId="48" r:id="rId8"/>
+    <sheet name="CanadaCheckOutRegression" sheetId="44" r:id="rId9"/>
+    <sheet name="KioskCheckOutRegression" sheetId="46" r:id="rId10"/>
+    <sheet name="CheckOutNegativeCasesRegression" sheetId="53" r:id="rId11"/>
+    <sheet name="EnvoyCheckOutRegression" sheetId="56" r:id="rId12"/>
+    <sheet name="PDPRegression" sheetId="29" r:id="rId13"/>
+    <sheet name="PLPRegression" sheetId="54" r:id="rId14"/>
+    <sheet name="MiniCartRegression" sheetId="57" r:id="rId15"/>
+    <sheet name="CartRegression" sheetId="49" r:id="rId16"/>
+    <sheet name="RegistrationRegression" sheetId="24" r:id="rId17"/>
+    <sheet name="MyAccountRegression" sheetId="27" r:id="rId18"/>
+    <sheet name="LoginRegression" sheetId="41" r:id="rId19"/>
+    <sheet name="CreateAccountsRegression" sheetId="52" r:id="rId20"/>
+    <sheet name="users" sheetId="13" r:id="rId21"/>
+    <sheet name="products" sheetId="55" r:id="rId22"/>
+    <sheet name="cards" sheetId="9" r:id="rId23"/>
+    <sheet name="addresses" sheetId="10" r:id="rId24"/>
+    <sheet name="VisualTestingCLPRegression" sheetId="42" r:id="rId25"/>
+    <sheet name="VisualTestingHPRegression" sheetId="40" r:id="rId26"/>
+    <sheet name="OrderHistoryRegression" sheetId="23" r:id="rId27"/>
+    <sheet name="QuickViewRegression" sheetId="39" r:id="rId28"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5194" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5256" uniqueCount="1021">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -3206,11 +3208,115 @@
   <si>
     <t>OH3</t>
   </si>
+  <si>
+    <t>HP1</t>
+  </si>
+  <si>
+    <t>check logo guest</t>
+  </si>
+  <si>
+    <t>verify
+logo</t>
+  </si>
+  <si>
+    <t>HP_Logo</t>
+  </si>
+  <si>
+    <t>HP2</t>
+  </si>
+  <si>
+    <t>HP3</t>
+  </si>
+  <si>
+    <t>check right header guest</t>
+  </si>
+  <si>
+    <t>verify RH for  United State</t>
+  </si>
+  <si>
+    <t>HP_RH_US</t>
+  </si>
+  <si>
+    <t>HP4</t>
+  </si>
+  <si>
+    <t>check right header guest internatinaly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verify RH for 
+internationally 
+</t>
+  </si>
+  <si>
+    <t>HP_RH_IU</t>
+  </si>
+  <si>
+    <t>HP5</t>
+  </si>
+  <si>
+    <t>check ship to US guest</t>
+  </si>
+  <si>
+    <t>verify ShipTo US</t>
+  </si>
+  <si>
+    <t>HP6</t>
+  </si>
+  <si>
+    <t>check ship to internatinally guest</t>
+  </si>
+  <si>
+    <t>verify ShipTo IU</t>
+  </si>
+  <si>
+    <t>HP7</t>
+  </si>
+  <si>
+    <t>check Myaccount for 
+US &amp; CAD users</t>
+  </si>
+  <si>
+    <t>verify MyAccountBttn for US and CAD users</t>
+  </si>
+  <si>
+    <t>HP8</t>
+  </si>
+  <si>
+    <t>check MyAccount for
+ internationally users</t>
+  </si>
+  <si>
+    <t>verify MyAccountBttn is
+ not all international users</t>
+  </si>
+  <si>
+    <t>HP9</t>
+  </si>
+  <si>
+    <t>update logo</t>
+  </si>
+  <si>
+    <t>HP10</t>
+  </si>
+  <si>
+    <t>HP11</t>
+  </si>
+  <si>
+    <t>update RH for  United State</t>
+  </si>
+  <si>
+    <t>HP12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> update RH for 
+internationally 
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -3497,7 +3603,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3892,6 +3998,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3991,6 +4113,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4026,6 +4165,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4201,55 +4357,1523 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47746A9-291E-4740-9134-AF5A1CD6645E}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="124" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="124" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="124" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="124" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="124"/>
+    <col min="6" max="6" width="19.5703125" style="124" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="124"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="109" t="s">
-        <v>726</v>
-      </c>
-      <c r="B1" s="109" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="110" t="s">
-        <v>727</v>
-      </c>
-      <c r="B2" s="111" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="108" t="s">
-        <v>728</v>
-      </c>
-      <c r="B3" s="112" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="108" t="s">
-        <v>729</v>
-      </c>
-      <c r="B4" s="112"/>
+      <c r="C1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="129" t="s">
+        <v>989</v>
+      </c>
+      <c r="B2" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>990</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>991</v>
+      </c>
+      <c r="E2" s="129"/>
+      <c r="F2" s="152" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="129" t="s">
+        <v>993</v>
+      </c>
+      <c r="B3" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" s="129"/>
+      <c r="F3" s="153" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="129" t="s">
+        <v>994</v>
+      </c>
+      <c r="B4" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>995</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>996</v>
+      </c>
+      <c r="E4" s="154"/>
+      <c r="F4" s="153" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45">
+      <c r="A5" s="129" t="s">
+        <v>998</v>
+      </c>
+      <c r="B5" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>999</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="129"/>
+      <c r="F5" s="152" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="129" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B6" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="155" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D6" s="155" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E6" s="125"/>
+      <c r="F6" s="156"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="129" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B7" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="155" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D7" s="155" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E7" s="125"/>
+      <c r="F7" s="156"/>
+    </row>
+    <row r="8" spans="1:6" ht="45">
+      <c r="A8" s="129" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B8" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="157" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D8" s="157" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E8" s="125"/>
+      <c r="F8" s="156"/>
+    </row>
+    <row r="9" spans="1:6" ht="60">
+      <c r="A9" s="129" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B9" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="157" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D9" s="157" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E9" s="125"/>
+      <c r="F9" s="156"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="129" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B10" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="70" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D10" s="70" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E10" s="129"/>
+      <c r="F10" s="152" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="129" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B11" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>303</v>
+      </c>
+      <c r="D11" s="70" t="s">
+        <v>303</v>
+      </c>
+      <c r="E11" s="129"/>
+      <c r="F11" s="153" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="129" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B12" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E12" s="154"/>
+      <c r="F12" s="153" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45">
+      <c r="A13" s="129" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B13" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E13" s="129"/>
+      <c r="F13" s="152" t="s">
+        <v>1001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="6" customFormat="1">
+      <c r="A1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A2" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="84"/>
+      <c r="K2" s="82" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A3" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="84"/>
+      <c r="K3" s="80" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A4" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="119"/>
+      <c r="C4" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="84"/>
+      <c r="K4" s="80" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A5" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="119"/>
+      <c r="C5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="84"/>
+      <c r="K5" s="80" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="75">
+      <c r="A6" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="119"/>
+      <c r="C6" s="18" t="s">
+        <v>461</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="J6" s="84"/>
+      <c r="K6" s="80" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A7" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="84"/>
+      <c r="K7" s="80" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A8" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="84"/>
+      <c r="K8" s="80" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A9" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="119"/>
+      <c r="C9" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="84"/>
+      <c r="K9" s="80" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A10" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="119"/>
+      <c r="C10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="84"/>
+      <c r="K10" s="80" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
+      <c r="A11" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" s="119"/>
+      <c r="C11" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="84"/>
+      <c r="K11" s="80" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="60">
+      <c r="A12" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="119"/>
+      <c r="C12" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="84"/>
+      <c r="K12" s="80" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60">
+      <c r="A13" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="119"/>
+      <c r="C13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="84"/>
+      <c r="K13" s="80" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="60">
+      <c r="A14" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>830</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="84"/>
+      <c r="K14" s="83"/>
+    </row>
+    <row r="15" spans="1:11" ht="60">
+      <c r="A15" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15" s="119"/>
+      <c r="C15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="86" t="s">
+        <v>830</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="84"/>
+      <c r="K15" s="83"/>
+    </row>
+    <row r="16" spans="1:11" ht="45">
+      <c r="A16" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="119"/>
+      <c r="C16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="86" t="s">
+        <v>830</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J16" s="84"/>
+      <c r="K16" s="83"/>
+    </row>
+    <row r="17" spans="1:11" ht="60">
+      <c r="A17" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" s="119"/>
+      <c r="C17" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="84"/>
+      <c r="K17" s="83"/>
+    </row>
+    <row r="18" spans="1:11" ht="45">
+      <c r="A18" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="D18" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="84"/>
+      <c r="K18" s="83"/>
+    </row>
+    <row r="19" spans="1:11" ht="45">
+      <c r="A19" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="119"/>
+      <c r="C19" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="84"/>
+      <c r="K19" s="83"/>
+    </row>
+    <row r="20" spans="1:11" ht="60">
+      <c r="A20" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B20" s="119"/>
+      <c r="C20" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="84"/>
+      <c r="K20" s="80" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60">
+      <c r="A21" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" s="119"/>
+      <c r="C21" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="84"/>
+      <c r="K21" s="80" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60">
+      <c r="A22" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" s="119"/>
+      <c r="C22" s="18" t="s">
+        <v>462</v>
+      </c>
+      <c r="D22" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22" s="84"/>
+      <c r="K22" s="80" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60">
+      <c r="A23" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" s="119"/>
+      <c r="C23" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="84"/>
+      <c r="K23" s="80" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="75">
+      <c r="A24" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B24" s="119"/>
+      <c r="C24" s="18" t="s">
+        <v>463</v>
+      </c>
+      <c r="D24" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="J24" s="84"/>
+      <c r="K24" s="80" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60">
+      <c r="A25" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B25" s="119"/>
+      <c r="C25" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="84"/>
+      <c r="K25" s="80" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60">
+      <c r="A26" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B26" s="119"/>
+      <c r="C26" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="84"/>
+      <c r="K26" s="80" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60">
+      <c r="A27" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27" s="119"/>
+      <c r="C27" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="84"/>
+      <c r="K27" s="80" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="60">
+      <c r="A28" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B28" s="119"/>
+      <c r="C28" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="84"/>
+      <c r="K28" s="80" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="60">
+      <c r="A29" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B29" s="119"/>
+      <c r="C29" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="84"/>
+      <c r="K29" s="80" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="60">
+      <c r="A30" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" s="119"/>
+      <c r="C30" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J30" s="84"/>
+      <c r="K30" s="80" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="60">
+      <c r="A31" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B31" s="119"/>
+      <c r="C31" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="84"/>
+      <c r="K31" s="80" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="60">
+      <c r="A32" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B32" s="119"/>
+      <c r="C32" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="84"/>
+      <c r="K32" s="83"/>
+    </row>
+    <row r="33" spans="1:11" ht="60">
+      <c r="A33" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B33" s="119"/>
+      <c r="C33" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33" s="84"/>
+      <c r="K33" s="83"/>
+    </row>
+    <row r="34" spans="1:11" ht="60">
+      <c r="A34" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34" s="119"/>
+      <c r="C34" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="84"/>
+      <c r="K34" s="83"/>
+    </row>
+    <row r="35" spans="1:11" ht="60">
+      <c r="A35" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B35" s="119"/>
+      <c r="C35" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="84"/>
+      <c r="K35" s="83"/>
+    </row>
+    <row r="36" spans="1:11" ht="60">
+      <c r="A36" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B36" s="119"/>
+      <c r="C36" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J36" s="84"/>
+      <c r="K36" s="83"/>
+    </row>
+    <row r="37" spans="1:11" ht="60">
+      <c r="A37" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B37" s="119"/>
+      <c r="C37" s="18" t="s">
+        <v>464</v>
+      </c>
+      <c r="D37" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J37" s="84"/>
+      <c r="K37" s="83"/>
+    </row>
+    <row r="38" spans="1:11" ht="45">
+      <c r="A38" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B38" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="84"/>
+      <c r="K38" s="83"/>
+    </row>
+    <row r="39" spans="1:11" ht="60">
+      <c r="A39" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>464</v>
+      </c>
+      <c r="D39" s="86" t="s">
+        <v>829</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J39" s="84"/>
+      <c r="K39" s="83"/>
+    </row>
+    <row r="40" spans="1:11" ht="60">
+      <c r="A40" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="B40" s="119"/>
+      <c r="C40" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="D40" s="86" t="s">
+        <v>326</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="84"/>
+      <c r="K40" s="82" t="s">
+        <v>531</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -5007,8 +6631,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -5126,16 +6750,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -5242,8 +6866,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -5490,8 +7114,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -5587,15 +7211,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6135,8 +7759,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet8">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6279,8 +7903,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet12">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6420,8 +8044,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6582,8 +8206,56 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="109" t="s">
+        <v>726</v>
+      </c>
+      <c r="B1" s="109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="110" t="s">
+        <v>727</v>
+      </c>
+      <c r="B2" s="111" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="108" t="s">
+        <v>728</v>
+      </c>
+      <c r="B3" s="112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="108" t="s">
+        <v>729</v>
+      </c>
+      <c r="B4" s="112"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6792,84 +8464,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="103" t="s">
-        <v>720</v>
-      </c>
-      <c r="B1" s="104" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="106" t="s">
-        <v>721</v>
-      </c>
-      <c r="B2" s="105" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="107" t="s">
-        <v>730</v>
-      </c>
-      <c r="B3" s="105" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="107" t="s">
-        <v>722</v>
-      </c>
-      <c r="B4" s="105" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="107" t="s">
-        <v>723</v>
-      </c>
-      <c r="B5" s="105" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="107" t="s">
-        <v>724</v>
-      </c>
-      <c r="B6" s="105" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="107" t="s">
-        <v>725</v>
-      </c>
-      <c r="B7" s="105"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -10609,24 +12205,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H88" r:id="rId1" display="tester011@cadtesting.com"/>
-    <hyperlink ref="H89" r:id="rId2" display="tester012@cadtesting.com"/>
-    <hyperlink ref="H90" r:id="rId3" display="tester013@cadtesting.com"/>
-    <hyperlink ref="H91" r:id="rId4" display="tester014@cadtesting.com"/>
-    <hyperlink ref="H92" r:id="rId5" display="tester015@cadtesting.com"/>
-    <hyperlink ref="H112" r:id="rId6" display="tester035@cadtesting.com"/>
-    <hyperlink ref="H93" r:id="rId7" display="tester016@cadtesting.com"/>
-    <hyperlink ref="H94" r:id="rId8" display="tester017@cadtesting.com"/>
-    <hyperlink ref="H2" r:id="rId9"/>
-    <hyperlink ref="H143" r:id="rId10"/>
+    <hyperlink ref="H88" r:id="rId1" display="tester011@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="H89" r:id="rId2" display="tester012@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
+    <hyperlink ref="H90" r:id="rId3" display="tester013@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000002000000}"/>
+    <hyperlink ref="H91" r:id="rId4" display="tester014@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000003000000}"/>
+    <hyperlink ref="H92" r:id="rId5" display="tester015@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000004000000}"/>
+    <hyperlink ref="H112" r:id="rId6" display="tester035@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000005000000}"/>
+    <hyperlink ref="H93" r:id="rId7" display="tester016@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000006000000}"/>
+    <hyperlink ref="H94" r:id="rId8" display="tester017@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000007000000}"/>
+    <hyperlink ref="H2" r:id="rId9" xr:uid="{00000000-0004-0000-1300-000008000000}"/>
+    <hyperlink ref="H143" r:id="rId10" xr:uid="{00000000-0004-0000-1300-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId11"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -11022,17 +12618,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M7" r:id="rId1"/>
-    <hyperlink ref="D11" r:id="rId2"/>
-    <hyperlink ref="D10" r:id="rId3"/>
+    <hyperlink ref="M7" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
+    <hyperlink ref="D10" r:id="rId3" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -11179,8 +12775,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr codeName="Sheet23">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -11469,8 +13065,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -11544,8 +13140,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -11683,14 +13279,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr codeName="Sheet7">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -11810,8 +13406,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -11936,7 +13532,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="103" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1" s="104" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="106" t="s">
+        <v>721</v>
+      </c>
+      <c r="B2" s="105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="107" t="s">
+        <v>730</v>
+      </c>
+      <c r="B3" s="105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="107" t="s">
+        <v>722</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="107" t="s">
+        <v>723</v>
+      </c>
+      <c r="B5" s="105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="107" t="s">
+        <v>724</v>
+      </c>
+      <c r="B6" s="105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="107" t="s">
+        <v>725</v>
+      </c>
+      <c r="B7" s="105"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet25">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -13626,8 +15298,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -15239,8 +16911,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -16930,8 +18602,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -18444,8 +20116,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -19764,15 +21436,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K40" r:id="rId1" display="tester035@ACVtesting.com"/>
+    <hyperlink ref="K40" r:id="rId1" display="tester035@ACVtesting.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -21093,1264 +22765,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:K40"/>
-  <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
-      <c r="A1" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A2" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="82" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A3" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="80" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A4" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="B4" s="119"/>
-      <c r="C4" s="18" t="s">
-        <v>460</v>
-      </c>
-      <c r="D4" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J4" s="84"/>
-      <c r="K4" s="80" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A5" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="119"/>
-      <c r="C5" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="84"/>
-      <c r="K5" s="80" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="75">
-      <c r="A6" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" s="119"/>
-      <c r="C6" s="18" t="s">
-        <v>461</v>
-      </c>
-      <c r="D6" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="80" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A7" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="119" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="80" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A8" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="B8" s="119" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="84"/>
-      <c r="K8" s="80" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A9" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B9" s="119"/>
-      <c r="C9" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="84"/>
-      <c r="K9" s="80" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A10" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="84"/>
-      <c r="K10" s="80" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
-      <c r="A11" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="84"/>
-      <c r="K11" s="80" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="60">
-      <c r="A12" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="B12" s="119"/>
-      <c r="C12" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="84"/>
-      <c r="K12" s="80" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="60">
-      <c r="A13" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="B13" s="119"/>
-      <c r="C13" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="84"/>
-      <c r="K13" s="80" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="60">
-      <c r="A14" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="B14" s="119" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="86" t="s">
-        <v>830</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="84"/>
-      <c r="K14" s="83"/>
-    </row>
-    <row r="15" spans="1:11" ht="60">
-      <c r="A15" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="86" t="s">
-        <v>830</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="84"/>
-      <c r="K15" s="83"/>
-    </row>
-    <row r="16" spans="1:11" ht="45">
-      <c r="A16" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="B16" s="119"/>
-      <c r="C16" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="86" t="s">
-        <v>830</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J16" s="84"/>
-      <c r="K16" s="83"/>
-    </row>
-    <row r="17" spans="1:11" ht="60">
-      <c r="A17" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="84"/>
-      <c r="K17" s="83"/>
-    </row>
-    <row r="18" spans="1:11" ht="45">
-      <c r="A18" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="B18" s="119" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>435</v>
-      </c>
-      <c r="D18" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="84"/>
-      <c r="K18" s="83"/>
-    </row>
-    <row r="19" spans="1:11" ht="45">
-      <c r="A19" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="B19" s="119"/>
-      <c r="C19" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" s="84"/>
-      <c r="K19" s="83"/>
-    </row>
-    <row r="20" spans="1:11" ht="60">
-      <c r="A20" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="84"/>
-      <c r="K20" s="80" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="60">
-      <c r="A21" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="B21" s="119"/>
-      <c r="C21" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="84"/>
-      <c r="K21" s="80" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="60">
-      <c r="A22" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B22" s="119"/>
-      <c r="C22" s="18" t="s">
-        <v>462</v>
-      </c>
-      <c r="D22" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J22" s="84"/>
-      <c r="K22" s="80" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60">
-      <c r="A23" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="B23" s="119"/>
-      <c r="C23" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J23" s="84"/>
-      <c r="K23" s="80" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="75">
-      <c r="A24" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B24" s="119"/>
-      <c r="C24" s="18" t="s">
-        <v>463</v>
-      </c>
-      <c r="D24" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="J24" s="84"/>
-      <c r="K24" s="80" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60">
-      <c r="A25" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B25" s="119"/>
-      <c r="C25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J25" s="84"/>
-      <c r="K25" s="80" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="60">
-      <c r="A26" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="B26" s="119"/>
-      <c r="C26" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="84"/>
-      <c r="K26" s="80" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="60">
-      <c r="A27" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J27" s="84"/>
-      <c r="K27" s="80" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="60">
-      <c r="A28" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="B28" s="119"/>
-      <c r="C28" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J28" s="84"/>
-      <c r="K28" s="80" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="60">
-      <c r="A29" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B29" s="119"/>
-      <c r="C29" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="84"/>
-      <c r="K29" s="80" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="60">
-      <c r="A30" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B30" s="119"/>
-      <c r="C30" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J30" s="84"/>
-      <c r="K30" s="80" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="60">
-      <c r="A31" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="B31" s="119"/>
-      <c r="C31" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J31" s="84"/>
-      <c r="K31" s="80" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="60">
-      <c r="A32" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B32" s="119"/>
-      <c r="C32" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J32" s="84"/>
-      <c r="K32" s="83"/>
-    </row>
-    <row r="33" spans="1:11" ht="60">
-      <c r="A33" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="B33" s="119"/>
-      <c r="C33" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J33" s="84"/>
-      <c r="K33" s="83"/>
-    </row>
-    <row r="34" spans="1:11" ht="60">
-      <c r="A34" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="B34" s="119"/>
-      <c r="C34" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="84"/>
-      <c r="K34" s="83"/>
-    </row>
-    <row r="35" spans="1:11" ht="60">
-      <c r="A35" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B35" s="119"/>
-      <c r="C35" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J35" s="84"/>
-      <c r="K35" s="83"/>
-    </row>
-    <row r="36" spans="1:11" ht="60">
-      <c r="A36" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="B36" s="119"/>
-      <c r="C36" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J36" s="84"/>
-      <c r="K36" s="83"/>
-    </row>
-    <row r="37" spans="1:11" ht="60">
-      <c r="A37" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="B37" s="119"/>
-      <c r="C37" s="18" t="s">
-        <v>464</v>
-      </c>
-      <c r="D37" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J37" s="84"/>
-      <c r="K37" s="83"/>
-    </row>
-    <row r="38" spans="1:11" ht="45">
-      <c r="A38" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="B38" s="119" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J38" s="84"/>
-      <c r="K38" s="83"/>
-    </row>
-    <row r="39" spans="1:11" ht="60">
-      <c r="A39" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="B39" s="119" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>464</v>
-      </c>
-      <c r="D39" s="86" t="s">
-        <v>829</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J39" s="84"/>
-      <c r="K39" s="83"/>
-    </row>
-    <row r="40" spans="1:11" ht="60">
-      <c r="A40" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="B40" s="119"/>
-      <c r="C40" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="D40" s="86" t="s">
-        <v>326</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J40" s="84"/>
-      <c r="K40" s="82" t="s">
-        <v>531</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
we did some changes on HomePage selectors and other changes on write email and confirm email  method
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{55E5EAD3-F920-446D-8968-DE0B5130CC15}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{80D537AC-97FD-435F-AF1D-5C9D5EE706ED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" firstSheet="18" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePageRegression" sheetId="58" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5269" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5275" uniqueCount="1039">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -3319,9 +3319,6 @@
     <t>P13</t>
   </si>
   <si>
-    <t>p12</t>
-  </si>
-  <si>
     <t>verify logo</t>
   </si>
   <si>
@@ -3344,6 +3341,24 @@
   </si>
   <si>
     <t>update RH for internationally</t>
+  </si>
+  <si>
+    <t>Send a piece of paradise with the gift of choice — a Tommy Bahama Gift Card! Available from $25-$1,000, it's delivered with an optional note and a custom-designed envelope ready for gifting. Gift Cards can be redeemed online, in our U.S. restaurants, retail stores and outlets.</t>
+  </si>
+  <si>
+    <t>Tommy Bahama Traditional Gift Card</t>
+  </si>
+  <si>
+    <t>GC0021</t>
+  </si>
+  <si>
+    <t>GC9900</t>
+  </si>
+  <si>
+    <t>Tommy Bahama Virtual Gift Card</t>
+  </si>
+  <si>
+    <t>Send a piece of paradise with the gift of choice—a Tommy Bahama Gift Card! Available from $25-$1,000, it's delivered via email, usually within 24 hours. Virtual Gift Cards can be redeemed online and in our restaurants, retail stores and outlets located in the U.S. and Canada.</t>
   </si>
 </sst>
 </file>
@@ -4022,7 +4037,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4031,6 +4045,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4380,7 +4397,7 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -4422,14 +4439,14 @@
       <c r="B2" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="149" t="s">
         <v>990</v>
       </c>
-      <c r="D2" s="150" t="s">
-        <v>1026</v>
+      <c r="D2" s="149" t="s">
+        <v>1025</v>
       </c>
       <c r="E2" s="107"/>
-      <c r="F2" s="151" t="s">
+      <c r="F2" s="150" t="s">
         <v>991</v>
       </c>
     </row>
@@ -4440,14 +4457,14 @@
       <c r="B3" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="150" t="s">
+      <c r="C3" s="149" t="s">
         <v>295</v>
       </c>
-      <c r="D3" s="150" t="s">
-        <v>1027</v>
+      <c r="D3" s="149" t="s">
+        <v>1026</v>
       </c>
       <c r="E3" s="107"/>
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="150" t="s">
         <v>301</v>
       </c>
     </row>
@@ -4458,14 +4475,14 @@
       <c r="B4" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="150" t="s">
+      <c r="C4" s="149" t="s">
         <v>994</v>
       </c>
-      <c r="D4" s="150" t="s">
-        <v>1028</v>
-      </c>
-      <c r="E4" s="152"/>
-      <c r="F4" s="151" t="s">
+      <c r="D4" s="149" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E4" s="151"/>
+      <c r="F4" s="150" t="s">
         <v>995</v>
       </c>
     </row>
@@ -4476,14 +4493,14 @@
       <c r="B5" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="150" t="s">
+      <c r="C5" s="149" t="s">
         <v>997</v>
       </c>
-      <c r="D5" s="150" t="s">
-        <v>1029</v>
+      <c r="D5" s="149" t="s">
+        <v>1028</v>
       </c>
       <c r="E5" s="107"/>
-      <c r="F5" s="151" t="s">
+      <c r="F5" s="150" t="s">
         <v>998</v>
       </c>
     </row>
@@ -4494,14 +4511,14 @@
       <c r="B6" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="150" t="s">
+      <c r="C6" s="149" t="s">
         <v>1000</v>
       </c>
-      <c r="D6" s="150" t="s">
+      <c r="D6" s="149" t="s">
         <v>1001</v>
       </c>
-      <c r="E6" s="153"/>
-      <c r="F6" s="153"/>
+      <c r="E6" s="152"/>
+      <c r="F6" s="152"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="107" t="s">
@@ -4510,14 +4527,14 @@
       <c r="B7" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="150" t="s">
+      <c r="C7" s="149" t="s">
         <v>1003</v>
       </c>
-      <c r="D7" s="150" t="s">
+      <c r="D7" s="149" t="s">
         <v>1004</v>
       </c>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="107" t="s">
@@ -4526,14 +4543,14 @@
       <c r="B8" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="150" t="s">
+      <c r="C8" s="149" t="s">
         <v>1006</v>
       </c>
-      <c r="D8" s="150" t="s">
+      <c r="D8" s="149" t="s">
         <v>1007</v>
       </c>
-      <c r="E8" s="153"/>
-      <c r="F8" s="153"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="152"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="107" t="s">
@@ -4542,14 +4559,14 @@
       <c r="B9" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="150" t="s">
+      <c r="C9" s="149" t="s">
         <v>1009</v>
       </c>
-      <c r="D9" s="150" t="s">
-        <v>1030</v>
-      </c>
-      <c r="E9" s="153"/>
-      <c r="F9" s="153"/>
+      <c r="D9" s="149" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E9" s="152"/>
+      <c r="F9" s="152"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="107" t="s">
@@ -4558,14 +4575,14 @@
       <c r="B10" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="150" t="s">
+      <c r="C10" s="149" t="s">
         <v>1011</v>
       </c>
-      <c r="D10" s="150" t="s">
+      <c r="D10" s="149" t="s">
         <v>1011</v>
       </c>
       <c r="E10" s="107"/>
-      <c r="F10" s="151" t="s">
+      <c r="F10" s="150" t="s">
         <v>991</v>
       </c>
     </row>
@@ -4576,14 +4593,14 @@
       <c r="B11" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="150" t="s">
+      <c r="C11" s="149" t="s">
         <v>303</v>
       </c>
-      <c r="D11" s="150" t="s">
-        <v>1031</v>
+      <c r="D11" s="149" t="s">
+        <v>1030</v>
       </c>
       <c r="E11" s="107"/>
-      <c r="F11" s="151" t="s">
+      <c r="F11" s="150" t="s">
         <v>301</v>
       </c>
     </row>
@@ -4594,18 +4611,18 @@
       <c r="B12" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="150" t="s">
-        <v>1032</v>
-      </c>
-      <c r="D12" s="150" t="s">
-        <v>1032</v>
-      </c>
-      <c r="E12" s="152"/>
-      <c r="F12" s="151" t="s">
+      <c r="C12" s="149" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D12" s="149" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E12" s="151"/>
+      <c r="F12" s="150" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6">
       <c r="A13" s="107" t="s">
         <v>1014</v>
       </c>
@@ -4613,13 +4630,13 @@
         <v>35</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E13" s="107"/>
-      <c r="F13" s="151" t="s">
+      <c r="F13" s="150" t="s">
         <v>998</v>
       </c>
     </row>
@@ -6783,7 +6800,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6885,7 +6902,7 @@
         <v>1021</v>
       </c>
       <c r="E5" s="146" t="s">
-        <v>1025</v>
+        <v>1015</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>834</v>
@@ -12288,8 +12305,8 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12680,39 +12697,55 @@
       <c r="A12" s="133" t="s">
         <v>1015</v>
       </c>
-      <c r="B12" s="134"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="40" t="s">
+      <c r="B12" s="134" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C12" s="102" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D12" s="153" t="s">
         <v>1023</v>
       </c>
-      <c r="E12" s="119"/>
-      <c r="F12" s="144"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="119">
-        <v>70</v>
-      </c>
-      <c r="J12" s="149"/>
-      <c r="K12" s="149"/>
-      <c r="L12" s="149"/>
-      <c r="M12" s="149"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102">
+        <v>75</v>
+      </c>
+      <c r="J12" s="102" t="s">
+        <v>1038</v>
+      </c>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
     </row>
     <row r="13" spans="1:13" ht="45">
       <c r="A13" s="133" t="s">
         <v>1024</v>
       </c>
-      <c r="B13" s="119"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="55" t="s">
+      <c r="B13" s="102" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C13" s="102" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D13" s="145" t="s">
         <v>1016</v>
       </c>
-      <c r="E13" s="119"/>
-      <c r="F13" s="119"/>
-      <c r="G13" s="119"/>
-      <c r="H13" s="119"/>
-      <c r="I13" s="119">
-        <v>70</v>
-      </c>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102">
+        <v>75</v>
+      </c>
+      <c r="J13" s="102" t="s">
+        <v>1033</v>
+      </c>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Home page Update, Runner Package
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{80D537AC-97FD-435F-AF1D-5C9D5EE706ED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" firstSheet="18" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HomePageRegression" sheetId="58" r:id="rId1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5275" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5268" uniqueCount="1039">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -3108,9 +3107,6 @@
     <t>TH31683</t>
   </si>
   <si>
-    <t>EMPFDXGROUND</t>
-  </si>
-  <si>
     <t>fresh
 new-user
 new-shipping
@@ -3360,11 +3356,14 @@
   <si>
     <t>Send a piece of paradise with the gift of choice—a Tommy Bahama Gift Card! Available from $25-$1,000, it's delivered via email, usually within 24 hours. Virtual Gift Cards can be redeemed online and in our restaurants, retail stores and outlets located in the U.S. and Canada.</t>
   </si>
+  <si>
+    <t>GROUND</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -4147,23 +4146,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4199,23 +4181,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4391,14 +4356,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47746A9-291E-4740-9134-AF5A1CD6645E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4434,34 +4399,30 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="107" t="s">
+        <v>988</v>
+      </c>
+      <c r="B2" s="107"/>
+      <c r="C2" s="149" t="s">
         <v>989</v>
       </c>
-      <c r="B2" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="149" t="s">
-        <v>990</v>
-      </c>
       <c r="D2" s="149" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E2" s="107"/>
       <c r="F2" s="150" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="107" t="s">
-        <v>992</v>
-      </c>
-      <c r="B3" s="107" t="s">
-        <v>35</v>
-      </c>
+        <v>991</v>
+      </c>
+      <c r="B3" s="107"/>
       <c r="C3" s="149" t="s">
         <v>295</v>
       </c>
       <c r="D3" s="149" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="E3" s="107"/>
       <c r="F3" s="150" t="s">
@@ -4470,125 +4431,113 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="107" t="s">
+        <v>992</v>
+      </c>
+      <c r="B4" s="107"/>
+      <c r="C4" s="149" t="s">
         <v>993</v>
       </c>
-      <c r="B4" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="149" t="s">
-        <v>994</v>
-      </c>
       <c r="D4" s="149" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E4" s="151"/>
       <c r="F4" s="150" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="107" t="s">
+        <v>995</v>
+      </c>
+      <c r="B5" s="107"/>
+      <c r="C5" s="149" t="s">
         <v>996</v>
       </c>
-      <c r="B5" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="149" t="s">
-        <v>997</v>
-      </c>
       <c r="D5" s="149" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E5" s="107"/>
       <c r="F5" s="150" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="107" t="s">
+        <v>998</v>
+      </c>
+      <c r="B6" s="107"/>
+      <c r="C6" s="149" t="s">
         <v>999</v>
       </c>
-      <c r="B6" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="149" t="s">
+      <c r="D6" s="149" t="s">
         <v>1000</v>
-      </c>
-      <c r="D6" s="149" t="s">
-        <v>1001</v>
       </c>
       <c r="E6" s="152"/>
       <c r="F6" s="152"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="107" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B7" s="107"/>
+      <c r="C7" s="149" t="s">
         <v>1002</v>
       </c>
-      <c r="B7" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="149" t="s">
+      <c r="D7" s="149" t="s">
         <v>1003</v>
-      </c>
-      <c r="D7" s="149" t="s">
-        <v>1004</v>
       </c>
       <c r="E7" s="152"/>
       <c r="F7" s="152"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="107" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B8" s="107"/>
+      <c r="C8" s="149" t="s">
         <v>1005</v>
       </c>
-      <c r="B8" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="149" t="s">
+      <c r="D8" s="149" t="s">
         <v>1006</v>
-      </c>
-      <c r="D8" s="149" t="s">
-        <v>1007</v>
       </c>
       <c r="E8" s="152"/>
       <c r="F8" s="152"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="107" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B9" s="107"/>
+      <c r="C9" s="149" t="s">
         <v>1008</v>
       </c>
-      <c r="B9" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="149" t="s">
-        <v>1009</v>
-      </c>
       <c r="D9" s="149" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E9" s="152"/>
       <c r="F9" s="152"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="107" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B10" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="149" t="s">
         <v>1010</v>
       </c>
-      <c r="B10" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="149" t="s">
-        <v>1011</v>
-      </c>
       <c r="D10" s="149" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E10" s="107"/>
       <c r="F10" s="150" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="107" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B11" s="107" t="s">
         <v>35</v>
@@ -4597,7 +4546,7 @@
         <v>303</v>
       </c>
       <c r="D11" s="149" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E11" s="107"/>
       <c r="F11" s="150" t="s">
@@ -4606,38 +4555,38 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="107" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B12" s="107" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="149" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D12" s="149" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E12" s="151"/>
       <c r="F12" s="150" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="107" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B13" s="107" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E13" s="107"/>
       <c r="F13" s="150" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
   </sheetData>
@@ -4647,7 +4596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -5907,7 +5856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6666,7 +6615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6733,7 +6682,7 @@
         <v>56</v>
       </c>
       <c r="D2" s="121" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>2</v>
@@ -6749,7 +6698,7 @@
         <v>636</v>
       </c>
       <c r="J2" s="135" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150">
@@ -6763,7 +6712,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="121" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>2</v>
@@ -6779,13 +6728,13 @@
         <v>28</v>
       </c>
       <c r="J3" s="135" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
@@ -6793,7 +6742,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6890,19 +6839,19 @@
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="86" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B5" s="86" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="146" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E5" s="146" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>834</v>
@@ -6911,19 +6860,19 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="86" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="146" t="s">
         <v>1018</v>
       </c>
-      <c r="B6" s="86" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="146" t="s">
+      <c r="D6" s="146" t="s">
         <v>1019</v>
       </c>
-      <c r="D6" s="146" t="s">
-        <v>1020</v>
-      </c>
       <c r="E6" s="146" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>834</v>
@@ -6932,7 +6881,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{D4E6D46B-9CBD-4B33-A01E-0070EE950B6B}"/>
+    <hyperlink ref="F5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
@@ -6940,7 +6889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7188,7 +7137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7231,7 +7180,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="91" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H1" s="91" t="s">
         <v>668</v>
@@ -7245,16 +7194,16 @@
         <v>35</v>
       </c>
       <c r="C2" s="93" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D2" s="93" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="E2" s="123" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="G2" s="107"/>
       <c r="H2" s="107"/>
@@ -7267,10 +7216,10 @@
         <v>35</v>
       </c>
       <c r="C3" s="93" t="s">
+        <v>969</v>
+      </c>
+      <c r="D3" s="93" t="s">
         <v>970</v>
-      </c>
-      <c r="D3" s="93" t="s">
-        <v>971</v>
       </c>
       <c r="E3" s="123" t="s">
         <v>175</v>
@@ -7284,7 +7233,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7292,7 +7241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7833,7 +7782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7977,7 +7926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -8118,7 +8067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -8280,7 +8229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -8328,7 +8277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -8538,7 +8487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -12252,7 +12201,7 @@
     </row>
     <row r="143" spans="1:8" ht="30">
       <c r="A143" s="87" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B143" s="88" t="s">
         <v>382</v>
@@ -12264,34 +12213,34 @@
         <v>384</v>
       </c>
       <c r="E143" s="87" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F143" s="88" t="s">
         <v>415</v>
       </c>
       <c r="G143" s="88" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="H143" s="136" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H88" r:id="rId1" display="tester011@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
-    <hyperlink ref="H89" r:id="rId2" display="tester012@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
-    <hyperlink ref="H90" r:id="rId3" display="tester013@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000002000000}"/>
-    <hyperlink ref="H91" r:id="rId4" display="tester014@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000003000000}"/>
-    <hyperlink ref="H92" r:id="rId5" display="tester015@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000004000000}"/>
-    <hyperlink ref="H112" r:id="rId6" display="tester035@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000005000000}"/>
-    <hyperlink ref="H93" r:id="rId7" display="tester016@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000006000000}"/>
-    <hyperlink ref="H94" r:id="rId8" display="tester017@cadtesting.com" xr:uid="{00000000-0004-0000-1300-000007000000}"/>
-    <hyperlink ref="H2" r:id="rId9" xr:uid="{00000000-0004-0000-1300-000008000000}"/>
-    <hyperlink ref="H143" r:id="rId10" xr:uid="{00000000-0004-0000-1300-000009000000}"/>
-    <hyperlink ref="H142" r:id="rId11" xr:uid="{19D3F54A-2F51-495F-BDB7-1FE40AA2AEC4}"/>
-    <hyperlink ref="H141" r:id="rId12" xr:uid="{3318D9D5-847D-46A6-BC6B-9FC759B6A7AA}"/>
-    <hyperlink ref="H139" r:id="rId13" xr:uid="{37B348EB-5EB3-4308-9352-78943741BC5B}"/>
-    <hyperlink ref="H140" r:id="rId14" xr:uid="{248F5444-CEDD-4569-8827-2A39D088668D}"/>
+    <hyperlink ref="H88" r:id="rId1" display="tester011@cadtesting.com"/>
+    <hyperlink ref="H89" r:id="rId2" display="tester012@cadtesting.com"/>
+    <hyperlink ref="H90" r:id="rId3" display="tester013@cadtesting.com"/>
+    <hyperlink ref="H91" r:id="rId4" display="tester014@cadtesting.com"/>
+    <hyperlink ref="H92" r:id="rId5" display="tester015@cadtesting.com"/>
+    <hyperlink ref="H112" r:id="rId6" display="tester035@cadtesting.com"/>
+    <hyperlink ref="H93" r:id="rId7" display="tester016@cadtesting.com"/>
+    <hyperlink ref="H94" r:id="rId8" display="tester017@cadtesting.com"/>
+    <hyperlink ref="H2" r:id="rId9"/>
+    <hyperlink ref="H143" r:id="rId10"/>
+    <hyperlink ref="H142" r:id="rId11"/>
+    <hyperlink ref="H141" r:id="rId12"/>
+    <hyperlink ref="H139" r:id="rId13"/>
+    <hyperlink ref="H140" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId15"/>
@@ -12299,14 +12248,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12428,7 +12377,7 @@
       </c>
       <c r="H3" s="81"/>
       <c r="I3" s="81" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="J3" s="122" t="s">
         <v>699</v>
@@ -12666,19 +12615,19 @@
     </row>
     <row r="11" spans="1:13" ht="60">
       <c r="A11" s="133" t="s">
+        <v>971</v>
+      </c>
+      <c r="B11" s="134" t="s">
+        <v>973</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>980</v>
+      </c>
+      <c r="D11" s="40" t="s">
         <v>972</v>
       </c>
-      <c r="B11" s="134" t="s">
-        <v>974</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>981</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>973</v>
-      </c>
       <c r="E11" s="119" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F11" s="144" t="s">
         <v>373</v>
@@ -12695,16 +12644,16 @@
     </row>
     <row r="12" spans="1:13" ht="31.5" customHeight="1">
       <c r="A12" s="133" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B12" s="134" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C12" s="102" t="s">
         <v>1036</v>
       </c>
-      <c r="C12" s="102" t="s">
-        <v>1037</v>
-      </c>
       <c r="D12" s="153" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="E12" s="102"/>
       <c r="F12" s="87"/>
@@ -12714,7 +12663,7 @@
         <v>75</v>
       </c>
       <c r="J12" s="102" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="K12" s="102"/>
       <c r="L12" s="102"/>
@@ -12722,16 +12671,16 @@
     </row>
     <row r="13" spans="1:13" ht="45">
       <c r="A13" s="133" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B13" s="102" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C13" s="102" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D13" s="145" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E13" s="102"/>
       <c r="F13" s="102"/>
@@ -12741,7 +12690,7 @@
         <v>75</v>
       </c>
       <c r="J13" s="102" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="K13" s="102"/>
       <c r="L13" s="102"/>
@@ -12749,9 +12698,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M7" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
-    <hyperlink ref="D11" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
+    <hyperlink ref="M7" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId2"/>
+    <hyperlink ref="D10" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -12759,7 +12708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -12907,7 +12856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -13030,13 +12979,13 @@
         <v>420</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F4" s="56" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="145" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="H4" s="56" t="s">
         <v>40</v>
@@ -13197,7 +13146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -13272,7 +13221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -13411,7 +13360,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -13470,7 +13419,7 @@
     </row>
     <row r="2" spans="1:11" ht="60">
       <c r="A2" s="39" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B2" s="39" t="s">
         <v>35</v>
@@ -13485,7 +13434,7 @@
         <v>507</v>
       </c>
       <c r="F2" s="88" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="G2" s="88" t="s">
         <v>422</v>
@@ -13503,7 +13452,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="39" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="2"/>
@@ -13518,7 +13467,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="39" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="2"/>
@@ -13538,7 +13487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -13663,14 +13612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13731,7 +13680,9 @@
       <c r="A7" s="101" t="s">
         <v>725</v>
       </c>
-      <c r="B7" s="99"/>
+      <c r="B7" s="99" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13739,14 +13690,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet25">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15430,7 +15381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -17043,7 +16994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -18734,14 +18685,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20130,7 +20081,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="73" t="s">
-        <v>960</v>
+        <v>1038</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>398</v>
@@ -20163,7 +20114,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="80" t="s">
-        <v>960</v>
+        <v>1038</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>15</v>
@@ -20187,10 +20138,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="121" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D45" s="121" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>43</v>
@@ -20218,10 +20169,10 @@
         <v>35</v>
       </c>
       <c r="C46" s="121" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D46" s="121" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>956</v>
@@ -20248,7 +20199,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -21567,7 +21518,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K40" r:id="rId1" display="tester035@ACVtesting.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="K40" r:id="rId1" display="tester035@ACVtesting.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
@@ -21575,14 +21526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B40"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21647,7 +21598,7 @@
         <v>39</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>2</v>
+        <v>983</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>953</v>
@@ -21680,7 +21631,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>954</v>
@@ -21713,7 +21664,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F4" s="121" t="s">
         <v>953</v>
@@ -21746,7 +21697,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F5" s="121" t="s">
         <v>954</v>
@@ -21779,7 +21730,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F6" s="121" t="s">
         <v>953</v>
@@ -21812,7 +21763,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F7" s="121" t="s">
         <v>954</v>
@@ -21845,7 +21796,7 @@
         <v>58</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F8" s="121" t="s">
         <v>953</v>
@@ -21878,7 +21829,7 @@
         <v>58</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F9" s="121" t="s">
         <v>954</v>
@@ -21911,7 +21862,7 @@
         <v>58</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F10" s="121" t="s">
         <v>953</v>
@@ -21944,7 +21895,7 @@
         <v>59</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F11" s="121" t="s">
         <v>954</v>
@@ -21977,7 +21928,7 @@
         <v>59</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F12" s="121" t="s">
         <v>953</v>
@@ -22010,7 +21961,7 @@
         <v>59</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F13" s="121" t="s">
         <v>954</v>
@@ -22043,7 +21994,7 @@
         <v>830</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F14" s="121" t="s">
         <v>953</v>
@@ -22105,7 +22056,7 @@
         <v>830</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F16" s="121" t="s">
         <v>953</v>
@@ -22198,7 +22149,7 @@
         <v>829</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F19" s="121" t="s">
         <v>953</v>
@@ -22229,7 +22180,7 @@
         <v>39</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F20" s="121" t="s">
         <v>953</v>
@@ -22262,7 +22213,7 @@
         <v>39</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F21" s="121" t="s">
         <v>953</v>
@@ -22295,7 +22246,7 @@
         <v>39</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F22" s="121" t="s">
         <v>953</v>
@@ -22328,7 +22279,7 @@
         <v>49</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F23" s="121" t="s">
         <v>953</v>
@@ -22361,7 +22312,7 @@
         <v>49</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F24" s="121" t="s">
         <v>953</v>
@@ -22394,7 +22345,7 @@
         <v>49</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F25" s="121" t="s">
         <v>953</v>
@@ -22427,7 +22378,7 @@
         <v>58</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F26" s="121" t="s">
         <v>953</v>
@@ -22460,7 +22411,7 @@
         <v>58</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F27" s="121" t="s">
         <v>953</v>
@@ -22493,7 +22444,7 @@
         <v>58</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F28" s="121" t="s">
         <v>953</v>
@@ -22559,7 +22510,7 @@
         <v>59</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F30" s="121" t="s">
         <v>953</v>
@@ -22592,7 +22543,7 @@
         <v>59</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F31" s="121" t="s">
         <v>953</v>
@@ -22625,7 +22576,7 @@
         <v>108</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F32" s="121" t="s">
         <v>953</v>
@@ -22656,7 +22607,7 @@
         <v>108</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F33" s="121" t="s">
         <v>953</v>
@@ -22687,7 +22638,7 @@
         <v>108</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F34" s="121" t="s">
         <v>954</v>
@@ -22718,7 +22669,7 @@
         <v>829</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F35" s="121" t="s">
         <v>954</v>
@@ -22749,7 +22700,7 @@
         <v>829</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F36" s="121" t="s">
         <v>954</v>
@@ -22780,7 +22731,7 @@
         <v>829</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>44</v>
+        <v>983</v>
       </c>
       <c r="F37" s="121" t="s">
         <v>954</v>

</xml_diff>

<commit_message>
New feature in search popup result Subscription popup
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="2955" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SearchRegression" sheetId="60" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5334" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5361" uniqueCount="1081">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -3368,9 +3368,6 @@
     <t>Search-1</t>
   </si>
   <si>
-    <t>Search results page with valid product</t>
-  </si>
-  <si>
     <t>shirt</t>
   </si>
   <si>
@@ -3394,9 +3391,6 @@
     <t>Search-3</t>
   </si>
   <si>
-    <t>Search results page with valid product and select currency</t>
-  </si>
-  <si>
     <t>Turkish Lira
 TRY</t>
   </si>
@@ -3407,27 +3401,18 @@
     <t>Search-4</t>
   </si>
   <si>
-    <t>Search results page with three character</t>
-  </si>
-  <si>
     <t>shi</t>
   </si>
   <si>
     <t>Search-5</t>
   </si>
   <si>
-    <t>Search results page with invalid product</t>
-  </si>
-  <si>
     <t>search</t>
   </si>
   <si>
     <t>Search-6</t>
   </si>
   <si>
-    <t>Search results page with empty search</t>
-  </si>
-  <si>
     <t>DDD</t>
   </si>
   <si>
@@ -3453,6 +3438,57 @@
   </si>
   <si>
     <t>https://www.tommybahama.com/en/Tommy-Bahama-Bird-of-Paradise-Gift-Card/p/GC0022-17181</t>
+  </si>
+  <si>
+    <t>Search results popup with valid product</t>
+  </si>
+  <si>
+    <t>Search results popup with valid product and select currency</t>
+  </si>
+  <si>
+    <t>Search results popup with three character only</t>
+  </si>
+  <si>
+    <t>Search results popup with a word that is not a product but the first three character give a valid products</t>
+  </si>
+  <si>
+    <t>Search results popup with invalid search</t>
+  </si>
+  <si>
+    <t>Search-7</t>
+  </si>
+  <si>
+    <t>Serach results popup with ID</t>
+  </si>
+  <si>
+    <t>OT317595</t>
+  </si>
+  <si>
+    <t>Mini_Cart</t>
+  </si>
+  <si>
+    <t>AccountSetup</t>
+  </si>
+  <si>
+    <t>checkoutNegativeRegression</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>OrderHistory</t>
+  </si>
+  <si>
+    <t>PLPRegression</t>
+  </si>
+  <si>
+    <t>QuickShopValidation</t>
+  </si>
+  <si>
+    <t>CreateNewAccounts</t>
+  </si>
+  <si>
+    <t>SearchRegression</t>
   </si>
 </sst>
 </file>
@@ -3466,13 +3502,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3487,7 +3523,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3710,7 +3746,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4076,14 +4112,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -4159,7 +4187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4194,7 +4222,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4409,29 +4437,29 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="9" style="82"/>
-    <col min="3" max="3" width="25.7109375" style="82" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="82" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="11.28515625" style="82" customWidth="1"/>
+    <col min="3" max="3" width="25.75" style="82" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" style="82" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="11.25" style="82" customWidth="1"/>
     <col min="10" max="16384" width="9" style="82"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="135" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="133" t="s">
+      <c r="C1" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="140" t="s">
+      <c r="D1" s="135" t="s">
         <v>912</v>
       </c>
       <c r="E1" s="135" t="s">
@@ -4450,154 +4478,172 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
-      <c r="A2" s="136" t="s">
+    <row r="2" spans="1:9" ht="28.5">
+      <c r="A2" s="137" t="s">
         <v>1040</v>
       </c>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="137" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="137" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D2" s="137" t="s">
         <v>1041</v>
-      </c>
-      <c r="D2" s="141" t="s">
-        <v>1042</v>
       </c>
       <c r="E2" s="137" t="s">
         <v>415</v>
       </c>
       <c r="F2" s="137" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G2" s="137" t="s">
         <v>1043</v>
-      </c>
-      <c r="G2" s="137" t="s">
-        <v>1044</v>
       </c>
       <c r="H2" s="137" t="s">
         <v>918</v>
       </c>
       <c r="I2" s="137" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="28.5">
+      <c r="A3" s="137" t="s">
         <v>1045</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30">
-      <c r="A3" s="136" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B3" s="136"/>
+      <c r="B3" s="137" t="s">
+        <v>35</v>
+      </c>
       <c r="C3" s="137" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D3" s="137" t="s">
         <v>1041</v>
-      </c>
-      <c r="D3" s="141" t="s">
-        <v>1042</v>
       </c>
       <c r="E3" s="137" t="s">
         <v>442</v>
       </c>
       <c r="F3" s="137" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G3" s="137" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="H3" s="137" t="s">
         <v>921</v>
       </c>
       <c r="I3" s="137"/>
     </row>
-    <row r="4" spans="1:9" ht="45">
-      <c r="A4" s="136" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B4" s="136"/>
+    <row r="4" spans="1:9" ht="42.75">
+      <c r="A4" s="137" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B4" s="137" t="s">
+        <v>35</v>
+      </c>
       <c r="C4" s="137" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D4" s="141" t="s">
-        <v>1042</v>
+        <v>1065</v>
+      </c>
+      <c r="D4" s="137" t="s">
+        <v>1041</v>
       </c>
       <c r="E4" s="137" t="s">
         <v>641</v>
       </c>
       <c r="F4" s="137" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="G4" s="137" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="H4" s="137"/>
       <c r="I4" s="137"/>
     </row>
-    <row r="5" spans="1:9" ht="30">
-      <c r="A5" s="136" t="s">
-        <v>1052</v>
-      </c>
-      <c r="B5" s="136"/>
+    <row r="5" spans="1:9" ht="28.5">
+      <c r="A5" s="137" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B5" s="137" t="s">
+        <v>35</v>
+      </c>
       <c r="C5" s="137" t="s">
-        <v>1053</v>
-      </c>
-      <c r="D5" s="141" t="s">
-        <v>1054</v>
+        <v>1066</v>
+      </c>
+      <c r="D5" s="137" t="s">
+        <v>1051</v>
       </c>
       <c r="E5" s="137"/>
       <c r="F5" s="137"/>
       <c r="G5" s="137" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="H5" s="137"/>
       <c r="I5" s="137"/>
     </row>
-    <row r="6" spans="1:9" ht="30">
-      <c r="A6" s="136" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B6" s="136"/>
+    <row r="6" spans="1:9" ht="57">
+      <c r="A6" s="137" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B6" s="137" t="s">
+        <v>35</v>
+      </c>
       <c r="C6" s="137" t="s">
-        <v>1056</v>
-      </c>
-      <c r="D6" s="141" t="s">
-        <v>1057</v>
+        <v>1067</v>
+      </c>
+      <c r="D6" s="137" t="s">
+        <v>1053</v>
       </c>
       <c r="E6" s="137" t="s">
         <v>415</v>
       </c>
       <c r="F6" s="137" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="G6" s="137" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="H6" s="137"/>
       <c r="I6" s="137"/>
     </row>
-    <row r="7" spans="1:9" ht="30">
-      <c r="A7" s="136" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B7" s="136"/>
+    <row r="7" spans="1:9" ht="28.5">
+      <c r="A7" s="137" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B7" s="137" t="s">
+        <v>35</v>
+      </c>
       <c r="C7" s="137" t="s">
-        <v>1059</v>
+        <v>1068</v>
       </c>
       <c r="D7" s="137" t="s">
-        <v>1060</v>
+        <v>1055</v>
       </c>
       <c r="E7" s="137"/>
       <c r="F7" s="137"/>
       <c r="G7" s="137" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="H7" s="137"/>
       <c r="I7" s="137"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="138"/>
-      <c r="B8" s="138"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
+      <c r="A8" s="137" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B8" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D8" s="137" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E8" s="137"/>
+      <c r="F8" s="137"/>
+      <c r="G8" s="137"/>
+      <c r="H8" s="137"/>
+      <c r="I8" s="137"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4616,20 +4662,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -4664,7 +4710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A2" s="14" t="s">
         <v>205</v>
       </c>
@@ -4697,7 +4743,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A3" s="14" t="s">
         <v>206</v>
       </c>
@@ -4730,7 +4776,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A4" s="14" t="s">
         <v>207</v>
       </c>
@@ -4763,7 +4809,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A5" s="14" t="s">
         <v>208</v>
       </c>
@@ -4796,7 +4842,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A6" s="14" t="s">
         <v>209</v>
       </c>
@@ -4829,7 +4875,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A7" s="14" t="s">
         <v>210</v>
       </c>
@@ -4862,7 +4908,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A8" s="14" t="s">
         <v>211</v>
       </c>
@@ -4895,7 +4941,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A9" s="14" t="s">
         <v>212</v>
       </c>
@@ -4928,7 +4974,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A10" s="14" t="s">
         <v>213</v>
       </c>
@@ -4961,7 +5007,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A11" s="14" t="s">
         <v>214</v>
       </c>
@@ -4994,7 +5040,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60">
+    <row r="12" spans="1:11" ht="57">
       <c r="A12" s="14" t="s">
         <v>215</v>
       </c>
@@ -5027,7 +5073,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60">
+    <row r="13" spans="1:11" ht="57">
       <c r="A13" s="14" t="s">
         <v>216</v>
       </c>
@@ -5060,7 +5106,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="60">
+    <row r="14" spans="1:11" ht="42.75">
       <c r="A14" s="14" t="s">
         <v>217</v>
       </c>
@@ -5091,7 +5137,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="50"/>
     </row>
-    <row r="15" spans="1:11" ht="60">
+    <row r="15" spans="1:11" ht="57">
       <c r="A15" s="14" t="s">
         <v>218</v>
       </c>
@@ -5122,7 +5168,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="50"/>
     </row>
-    <row r="16" spans="1:11" ht="45">
+    <row r="16" spans="1:11" ht="42.75">
       <c r="A16" s="14" t="s">
         <v>219</v>
       </c>
@@ -5153,7 +5199,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="50"/>
     </row>
-    <row r="17" spans="1:11" ht="60">
+    <row r="17" spans="1:11" ht="57">
       <c r="A17" s="14" t="s">
         <v>220</v>
       </c>
@@ -5184,7 +5230,7 @@
       <c r="J17" s="19"/>
       <c r="K17" s="50"/>
     </row>
-    <row r="18" spans="1:11" ht="60">
+    <row r="18" spans="1:11" ht="57">
       <c r="A18" s="14" t="s">
         <v>221</v>
       </c>
@@ -5215,7 +5261,7 @@
       <c r="J18" s="19"/>
       <c r="K18" s="50"/>
     </row>
-    <row r="19" spans="1:11" ht="60">
+    <row r="19" spans="1:11" ht="57">
       <c r="A19" s="14" t="s">
         <v>222</v>
       </c>
@@ -5246,7 +5292,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="50"/>
     </row>
-    <row r="20" spans="1:11" ht="60">
+    <row r="20" spans="1:11" ht="57">
       <c r="A20" s="14" t="s">
         <v>223</v>
       </c>
@@ -5279,7 +5325,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="60">
+    <row r="21" spans="1:11" ht="57">
       <c r="A21" s="14" t="s">
         <v>224</v>
       </c>
@@ -5312,7 +5358,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60">
+    <row r="22" spans="1:11" ht="57">
       <c r="A22" s="14" t="s">
         <v>225</v>
       </c>
@@ -5345,7 +5391,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="60">
+    <row r="23" spans="1:11" ht="57">
       <c r="A23" s="14" t="s">
         <v>226</v>
       </c>
@@ -5378,7 +5424,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="60">
+    <row r="24" spans="1:11" ht="57">
       <c r="A24" s="14" t="s">
         <v>227</v>
       </c>
@@ -5411,7 +5457,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="60">
+    <row r="25" spans="1:11" ht="57">
       <c r="A25" s="14" t="s">
         <v>228</v>
       </c>
@@ -5444,7 +5490,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60">
+    <row r="26" spans="1:11" ht="57">
       <c r="A26" s="14" t="s">
         <v>229</v>
       </c>
@@ -5477,7 +5523,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="60">
+    <row r="27" spans="1:11" ht="57">
       <c r="A27" s="14" t="s">
         <v>230</v>
       </c>
@@ -5510,7 +5556,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60">
+    <row r="28" spans="1:11" ht="57">
       <c r="A28" s="14" t="s">
         <v>231</v>
       </c>
@@ -5543,7 +5589,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60">
+    <row r="29" spans="1:11" ht="57">
       <c r="A29" s="14" t="s">
         <v>232</v>
       </c>
@@ -5576,7 +5622,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60">
+    <row r="30" spans="1:11" ht="57">
       <c r="A30" s="14" t="s">
         <v>233</v>
       </c>
@@ -5609,7 +5655,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="60">
+    <row r="31" spans="1:11" ht="57">
       <c r="A31" s="14" t="s">
         <v>234</v>
       </c>
@@ -5642,7 +5688,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="60">
+    <row r="32" spans="1:11" ht="57">
       <c r="A32" s="14" t="s">
         <v>235</v>
       </c>
@@ -5673,7 +5719,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="50"/>
     </row>
-    <row r="33" spans="1:11" ht="60">
+    <row r="33" spans="1:11" ht="57">
       <c r="A33" s="14" t="s">
         <v>236</v>
       </c>
@@ -5704,7 +5750,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="50"/>
     </row>
-    <row r="34" spans="1:11" ht="60">
+    <row r="34" spans="1:11" ht="57">
       <c r="A34" s="14" t="s">
         <v>237</v>
       </c>
@@ -5735,7 +5781,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="50"/>
     </row>
-    <row r="35" spans="1:11" ht="60">
+    <row r="35" spans="1:11" ht="57">
       <c r="A35" s="14" t="s">
         <v>238</v>
       </c>
@@ -5766,7 +5812,7 @@
       <c r="J35" s="19"/>
       <c r="K35" s="50"/>
     </row>
-    <row r="36" spans="1:11" ht="60">
+    <row r="36" spans="1:11" ht="57">
       <c r="A36" s="14" t="s">
         <v>239</v>
       </c>
@@ -5797,7 +5843,7 @@
       <c r="J36" s="19"/>
       <c r="K36" s="50"/>
     </row>
-    <row r="37" spans="1:11" ht="60">
+    <row r="37" spans="1:11" ht="57">
       <c r="A37" s="14" t="s">
         <v>240</v>
       </c>
@@ -5828,7 +5874,7 @@
       <c r="J37" s="19"/>
       <c r="K37" s="50"/>
     </row>
-    <row r="38" spans="1:11" ht="60">
+    <row r="38" spans="1:11" ht="57">
       <c r="A38" s="14" t="s">
         <v>241</v>
       </c>
@@ -5859,7 +5905,7 @@
       <c r="J38" s="19"/>
       <c r="K38" s="50"/>
     </row>
-    <row r="39" spans="1:11" ht="60">
+    <row r="39" spans="1:11" ht="57">
       <c r="A39" s="14" t="s">
         <v>281</v>
       </c>
@@ -5890,7 +5936,7 @@
       <c r="J39" s="19"/>
       <c r="K39" s="50"/>
     </row>
-    <row r="40" spans="1:11" ht="60">
+    <row r="40" spans="1:11" ht="57">
       <c r="A40" s="14" t="s">
         <v>324</v>
       </c>
@@ -5943,20 +5989,20 @@
       <selection activeCell="B2" sqref="B2:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -5991,7 +6037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A2" s="14" t="s">
         <v>205</v>
       </c>
@@ -6024,7 +6070,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A3" s="14" t="s">
         <v>206</v>
       </c>
@@ -6057,7 +6103,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A4" s="14" t="s">
         <v>207</v>
       </c>
@@ -6090,7 +6136,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A5" s="14" t="s">
         <v>208</v>
       </c>
@@ -6123,7 +6169,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="75">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="71.25">
       <c r="A6" s="14" t="s">
         <v>209</v>
       </c>
@@ -6156,7 +6202,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A7" s="14" t="s">
         <v>210</v>
       </c>
@@ -6189,7 +6235,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A8" s="14" t="s">
         <v>211</v>
       </c>
@@ -6222,7 +6268,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A9" s="14" t="s">
         <v>212</v>
       </c>
@@ -6255,7 +6301,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A10" s="14" t="s">
         <v>213</v>
       </c>
@@ -6288,7 +6334,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A11" s="14" t="s">
         <v>214</v>
       </c>
@@ -6321,7 +6367,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60">
+    <row r="12" spans="1:11" ht="57">
       <c r="A12" s="14" t="s">
         <v>215</v>
       </c>
@@ -6354,7 +6400,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60">
+    <row r="13" spans="1:11" ht="57">
       <c r="A13" s="14" t="s">
         <v>216</v>
       </c>
@@ -6387,7 +6433,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="60">
+    <row r="14" spans="1:11" ht="42.75">
       <c r="A14" s="14" t="s">
         <v>217</v>
       </c>
@@ -6418,7 +6464,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="50"/>
     </row>
-    <row r="15" spans="1:11" ht="60">
+    <row r="15" spans="1:11" ht="57">
       <c r="A15" s="14" t="s">
         <v>218</v>
       </c>
@@ -6449,7 +6495,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="50"/>
     </row>
-    <row r="16" spans="1:11" ht="60">
+    <row r="16" spans="1:11" ht="42.75">
       <c r="A16" s="14" t="s">
         <v>219</v>
       </c>
@@ -6480,7 +6526,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="50"/>
     </row>
-    <row r="17" spans="1:11" ht="60">
+    <row r="17" spans="1:11" ht="57">
       <c r="A17" s="14" t="s">
         <v>220</v>
       </c>
@@ -6511,7 +6557,7 @@
       <c r="J17" s="19"/>
       <c r="K17" s="50"/>
     </row>
-    <row r="18" spans="1:11" ht="45">
+    <row r="18" spans="1:11" ht="42.75">
       <c r="A18" s="14" t="s">
         <v>221</v>
       </c>
@@ -6542,7 +6588,7 @@
       <c r="J18" s="19"/>
       <c r="K18" s="50"/>
     </row>
-    <row r="19" spans="1:11" ht="60">
+    <row r="19" spans="1:11" ht="57">
       <c r="A19" s="14" t="s">
         <v>222</v>
       </c>
@@ -6573,7 +6619,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="50"/>
     </row>
-    <row r="20" spans="1:11" ht="60">
+    <row r="20" spans="1:11" ht="57">
       <c r="A20" s="14" t="s">
         <v>223</v>
       </c>
@@ -6606,7 +6652,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="60">
+    <row r="21" spans="1:11" ht="57">
       <c r="A21" s="14" t="s">
         <v>224</v>
       </c>
@@ -6639,7 +6685,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60">
+    <row r="22" spans="1:11" ht="57">
       <c r="A22" s="14" t="s">
         <v>225</v>
       </c>
@@ -6672,7 +6718,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="60">
+    <row r="23" spans="1:11" ht="57">
       <c r="A23" s="14" t="s">
         <v>226</v>
       </c>
@@ -6705,7 +6751,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="75">
+    <row r="24" spans="1:11" ht="71.25">
       <c r="A24" s="14" t="s">
         <v>227</v>
       </c>
@@ -6738,7 +6784,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="60">
+    <row r="25" spans="1:11" ht="57">
       <c r="A25" s="14" t="s">
         <v>228</v>
       </c>
@@ -6771,7 +6817,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60">
+    <row r="26" spans="1:11" ht="57">
       <c r="A26" s="14" t="s">
         <v>229</v>
       </c>
@@ -6804,7 +6850,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="60">
+    <row r="27" spans="1:11" ht="57">
       <c r="A27" s="14" t="s">
         <v>230</v>
       </c>
@@ -6837,7 +6883,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60">
+    <row r="28" spans="1:11" ht="57">
       <c r="A28" s="14" t="s">
         <v>231</v>
       </c>
@@ -6870,7 +6916,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60">
+    <row r="29" spans="1:11" ht="57">
       <c r="A29" s="14" t="s">
         <v>232</v>
       </c>
@@ -6903,7 +6949,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60">
+    <row r="30" spans="1:11" ht="57">
       <c r="A30" s="14" t="s">
         <v>233</v>
       </c>
@@ -6936,7 +6982,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="60">
+    <row r="31" spans="1:11" ht="57">
       <c r="A31" s="14" t="s">
         <v>234</v>
       </c>
@@ -6969,7 +7015,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="60">
+    <row r="32" spans="1:11" ht="57">
       <c r="A32" s="14" t="s">
         <v>235</v>
       </c>
@@ -7000,7 +7046,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="50"/>
     </row>
-    <row r="33" spans="1:11" ht="60">
+    <row r="33" spans="1:11" ht="57">
       <c r="A33" s="14" t="s">
         <v>236</v>
       </c>
@@ -7031,7 +7077,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="50"/>
     </row>
-    <row r="34" spans="1:11" ht="60">
+    <row r="34" spans="1:11" ht="57">
       <c r="A34" s="14" t="s">
         <v>237</v>
       </c>
@@ -7062,7 +7108,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="50"/>
     </row>
-    <row r="35" spans="1:11" ht="60">
+    <row r="35" spans="1:11" ht="57">
       <c r="A35" s="14" t="s">
         <v>238</v>
       </c>
@@ -7093,7 +7139,7 @@
       <c r="J35" s="19"/>
       <c r="K35" s="50"/>
     </row>
-    <row r="36" spans="1:11" ht="60">
+    <row r="36" spans="1:11" ht="57">
       <c r="A36" s="14" t="s">
         <v>239</v>
       </c>
@@ -7124,7 +7170,7 @@
       <c r="J36" s="19"/>
       <c r="K36" s="50"/>
     </row>
-    <row r="37" spans="1:11" ht="60">
+    <row r="37" spans="1:11" ht="57">
       <c r="A37" s="14" t="s">
         <v>240</v>
       </c>
@@ -7155,7 +7201,7 @@
       <c r="J37" s="19"/>
       <c r="K37" s="50"/>
     </row>
-    <row r="38" spans="1:11" ht="45">
+    <row r="38" spans="1:11" ht="42.75">
       <c r="A38" s="14" t="s">
         <v>241</v>
       </c>
@@ -7186,7 +7232,7 @@
       <c r="J38" s="19"/>
       <c r="K38" s="50"/>
     </row>
-    <row r="39" spans="1:11" ht="60">
+    <row r="39" spans="1:11" ht="57">
       <c r="A39" s="14" t="s">
         <v>281</v>
       </c>
@@ -7217,7 +7263,7 @@
       <c r="J39" s="19"/>
       <c r="K39" s="50"/>
     </row>
-    <row r="40" spans="1:11" ht="60">
+    <row r="40" spans="1:11" ht="57">
       <c r="A40" s="14" t="s">
         <v>324</v>
       </c>
@@ -7267,20 +7313,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -7315,7 +7361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A2" s="14" t="s">
         <v>205</v>
       </c>
@@ -7348,7 +7394,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A3" s="14" t="s">
         <v>206</v>
       </c>
@@ -7379,7 +7425,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A4" s="14" t="s">
         <v>207</v>
       </c>
@@ -7410,7 +7456,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A5" s="14" t="s">
         <v>208</v>
       </c>
@@ -7441,7 +7487,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="75">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="71.25">
       <c r="A6" s="14" t="s">
         <v>209</v>
       </c>
@@ -7472,7 +7518,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A7" s="14" t="s">
         <v>210</v>
       </c>
@@ -7505,7 +7551,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A8" s="14" t="s">
         <v>211</v>
       </c>
@@ -7538,7 +7584,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A9" s="14" t="s">
         <v>212</v>
       </c>
@@ -7569,7 +7615,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A10" s="14" t="s">
         <v>213</v>
       </c>
@@ -7600,7 +7646,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A11" s="14" t="s">
         <v>214</v>
       </c>
@@ -7631,7 +7677,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60">
+    <row r="12" spans="1:11" ht="57">
       <c r="A12" s="14" t="s">
         <v>215</v>
       </c>
@@ -7662,7 +7708,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60">
+    <row r="13" spans="1:11" ht="57">
       <c r="A13" s="14" t="s">
         <v>216</v>
       </c>
@@ -7693,7 +7739,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="60">
+    <row r="14" spans="1:11" ht="42.75">
       <c r="A14" s="14" t="s">
         <v>217</v>
       </c>
@@ -7724,7 +7770,7 @@
       <c r="J14" s="76"/>
       <c r="K14" s="75"/>
     </row>
-    <row r="15" spans="1:11" ht="60">
+    <row r="15" spans="1:11" ht="57">
       <c r="A15" s="14" t="s">
         <v>218</v>
       </c>
@@ -7753,7 +7799,7 @@
       <c r="J15" s="76"/>
       <c r="K15" s="75"/>
     </row>
-    <row r="16" spans="1:11" ht="45">
+    <row r="16" spans="1:11" ht="42.75">
       <c r="A16" s="14" t="s">
         <v>219</v>
       </c>
@@ -7782,7 +7828,7 @@
       <c r="J16" s="76"/>
       <c r="K16" s="75"/>
     </row>
-    <row r="17" spans="1:11" ht="60">
+    <row r="17" spans="1:11" ht="57">
       <c r="A17" s="14" t="s">
         <v>220</v>
       </c>
@@ -7811,7 +7857,7 @@
       <c r="J17" s="76"/>
       <c r="K17" s="75"/>
     </row>
-    <row r="18" spans="1:11" ht="45">
+    <row r="18" spans="1:11" ht="42.75">
       <c r="A18" s="14" t="s">
         <v>221</v>
       </c>
@@ -7842,7 +7888,7 @@
       <c r="J18" s="76"/>
       <c r="K18" s="75"/>
     </row>
-    <row r="19" spans="1:11" ht="45">
+    <row r="19" spans="1:11" ht="42.75">
       <c r="A19" s="14" t="s">
         <v>222</v>
       </c>
@@ -7871,7 +7917,7 @@
       <c r="J19" s="76"/>
       <c r="K19" s="75"/>
     </row>
-    <row r="20" spans="1:11" ht="60">
+    <row r="20" spans="1:11" ht="57">
       <c r="A20" s="14" t="s">
         <v>223</v>
       </c>
@@ -7902,7 +7948,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="60">
+    <row r="21" spans="1:11" ht="57">
       <c r="A21" s="14" t="s">
         <v>224</v>
       </c>
@@ -7933,7 +7979,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60">
+    <row r="22" spans="1:11" ht="57">
       <c r="A22" s="14" t="s">
         <v>225</v>
       </c>
@@ -7964,7 +8010,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="60">
+    <row r="23" spans="1:11" ht="57">
       <c r="A23" s="14" t="s">
         <v>226</v>
       </c>
@@ -7995,7 +8041,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="75">
+    <row r="24" spans="1:11" ht="71.25">
       <c r="A24" s="14" t="s">
         <v>227</v>
       </c>
@@ -8026,7 +8072,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="60">
+    <row r="25" spans="1:11" ht="57">
       <c r="A25" s="14" t="s">
         <v>228</v>
       </c>
@@ -8057,7 +8103,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60">
+    <row r="26" spans="1:11" ht="57">
       <c r="A26" s="14" t="s">
         <v>229</v>
       </c>
@@ -8088,7 +8134,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="60">
+    <row r="27" spans="1:11" ht="57">
       <c r="A27" s="14" t="s">
         <v>230</v>
       </c>
@@ -8119,7 +8165,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60">
+    <row r="28" spans="1:11" ht="57">
       <c r="A28" s="14" t="s">
         <v>231</v>
       </c>
@@ -8150,7 +8196,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60">
+    <row r="29" spans="1:11" ht="57">
       <c r="A29" s="14" t="s">
         <v>232</v>
       </c>
@@ -8181,7 +8227,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60">
+    <row r="30" spans="1:11" ht="57">
       <c r="A30" s="14" t="s">
         <v>233</v>
       </c>
@@ -8212,7 +8258,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="60">
+    <row r="31" spans="1:11" ht="57">
       <c r="A31" s="14" t="s">
         <v>234</v>
       </c>
@@ -8243,7 +8289,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="60">
+    <row r="32" spans="1:11" ht="57">
       <c r="A32" s="14" t="s">
         <v>235</v>
       </c>
@@ -8272,7 +8318,7 @@
       <c r="J32" s="76"/>
       <c r="K32" s="75"/>
     </row>
-    <row r="33" spans="1:11" ht="60">
+    <row r="33" spans="1:11" ht="57">
       <c r="A33" s="14" t="s">
         <v>236</v>
       </c>
@@ -8301,7 +8347,7 @@
       <c r="J33" s="76"/>
       <c r="K33" s="75"/>
     </row>
-    <row r="34" spans="1:11" ht="60">
+    <row r="34" spans="1:11" ht="57">
       <c r="A34" s="14" t="s">
         <v>237</v>
       </c>
@@ -8330,7 +8376,7 @@
       <c r="J34" s="76"/>
       <c r="K34" s="75"/>
     </row>
-    <row r="35" spans="1:11" ht="60">
+    <row r="35" spans="1:11" ht="57">
       <c r="A35" s="14" t="s">
         <v>238</v>
       </c>
@@ -8359,7 +8405,7 @@
       <c r="J35" s="76"/>
       <c r="K35" s="75"/>
     </row>
-    <row r="36" spans="1:11" ht="60">
+    <row r="36" spans="1:11" ht="57">
       <c r="A36" s="14" t="s">
         <v>239</v>
       </c>
@@ -8388,7 +8434,7 @@
       <c r="J36" s="76"/>
       <c r="K36" s="75"/>
     </row>
-    <row r="37" spans="1:11" ht="60">
+    <row r="37" spans="1:11" ht="57">
       <c r="A37" s="14" t="s">
         <v>240</v>
       </c>
@@ -8417,7 +8463,7 @@
       <c r="J37" s="76"/>
       <c r="K37" s="75"/>
     </row>
-    <row r="38" spans="1:11" ht="45">
+    <row r="38" spans="1:11" ht="42.75">
       <c r="A38" s="14" t="s">
         <v>241</v>
       </c>
@@ -8448,7 +8494,7 @@
       <c r="J38" s="76"/>
       <c r="K38" s="75"/>
     </row>
-    <row r="39" spans="1:11" ht="60">
+    <row r="39" spans="1:11" ht="57">
       <c r="A39" s="14" t="s">
         <v>281</v>
       </c>
@@ -8479,7 +8525,7 @@
       <c r="J39" s="76"/>
       <c r="K39" s="75"/>
     </row>
-    <row r="40" spans="1:11" ht="60">
+    <row r="40" spans="1:11" ht="57">
       <c r="A40" s="14" t="s">
         <v>324</v>
       </c>
@@ -8527,11 +8573,11 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="10" max="10" width="34.625" customWidth="1"/>
     <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8570,7 +8616,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60">
+    <row r="2" spans="1:11" ht="42.75">
       <c r="A2" s="118" t="s">
         <v>854</v>
       </c>
@@ -8605,7 +8651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60">
+    <row r="3" spans="1:11" ht="42.75">
       <c r="A3" s="118" t="s">
         <v>855</v>
       </c>
@@ -8640,7 +8686,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60">
+    <row r="4" spans="1:11" ht="42.75">
       <c r="A4" s="118" t="s">
         <v>856</v>
       </c>
@@ -8675,7 +8721,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="60">
+    <row r="5" spans="1:11" ht="42.75">
       <c r="A5" s="118" t="s">
         <v>857</v>
       </c>
@@ -8710,7 +8756,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="60">
+    <row r="6" spans="1:11" ht="42.75">
       <c r="A6" s="118" t="s">
         <v>858</v>
       </c>
@@ -8745,7 +8791,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60">
+    <row r="7" spans="1:11" ht="42.75">
       <c r="A7" s="118" t="s">
         <v>859</v>
       </c>
@@ -8780,7 +8826,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60">
+    <row r="8" spans="1:11" ht="42.75">
       <c r="A8" s="118" t="s">
         <v>860</v>
       </c>
@@ -8815,7 +8861,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60">
+    <row r="9" spans="1:11" ht="42.75">
       <c r="A9" s="118" t="s">
         <v>861</v>
       </c>
@@ -8850,7 +8896,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="60">
+    <row r="10" spans="1:11" ht="42.75">
       <c r="A10" s="118" t="s">
         <v>862</v>
       </c>
@@ -8885,7 +8931,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="60">
+    <row r="11" spans="1:11" ht="42.75">
       <c r="A11" s="118" t="s">
         <v>863</v>
       </c>
@@ -8920,7 +8966,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60">
+    <row r="12" spans="1:11" ht="42.75">
       <c r="A12" s="118" t="s">
         <v>864</v>
       </c>
@@ -8955,7 +9001,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60">
+    <row r="13" spans="1:11" ht="42.75">
       <c r="A13" s="118" t="s">
         <v>865</v>
       </c>
@@ -8990,7 +9036,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="60">
+    <row r="14" spans="1:11" ht="42.75">
       <c r="A14" s="118" t="s">
         <v>866</v>
       </c>
@@ -9025,7 +9071,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="60">
+    <row r="15" spans="1:11" ht="42.75">
       <c r="A15" s="118" t="s">
         <v>867</v>
       </c>
@@ -9060,7 +9106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="60">
+    <row r="16" spans="1:11" ht="42.75">
       <c r="A16" s="118" t="s">
         <v>868</v>
       </c>
@@ -9095,7 +9141,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="60">
+    <row r="17" spans="1:11" ht="42.75">
       <c r="A17" s="118" t="s">
         <v>869</v>
       </c>
@@ -9130,7 +9176,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45">
+    <row r="18" spans="1:11" ht="42.75">
       <c r="A18" s="118" t="s">
         <v>870</v>
       </c>
@@ -9165,7 +9211,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45">
+    <row r="19" spans="1:11" ht="42.75">
       <c r="A19" s="118" t="s">
         <v>871</v>
       </c>
@@ -9200,7 +9246,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45">
+    <row r="20" spans="1:11" ht="42.75">
       <c r="A20" s="118" t="s">
         <v>872</v>
       </c>
@@ -9235,7 +9281,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45">
+    <row r="21" spans="1:11" ht="42.75">
       <c r="A21" s="118" t="s">
         <v>873</v>
       </c>
@@ -9286,21 +9332,21 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="113"/>
-    <col min="3" max="3" width="9.5703125" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.85546875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.28515625" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" style="113" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.125" style="113"/>
+    <col min="3" max="3" width="9.625" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.625" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.25" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.875" style="113" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28" style="113" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="113"/>
+    <col min="11" max="16384" width="9.125" style="113"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -9332,7 +9378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="150">
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="142.5">
       <c r="A2" s="84" t="s">
         <v>205</v>
       </c>
@@ -9362,7 +9408,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="150">
+    <row r="3" spans="1:10" ht="142.5">
       <c r="A3" s="84" t="s">
         <v>206</v>
       </c>
@@ -9409,22 +9455,22 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.375" customWidth="1"/>
+    <col min="5" max="5" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="20" t="s">
         <v>53</v>
       </c>
@@ -9447,7 +9493,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90">
+    <row r="2" spans="1:7" ht="85.5">
       <c r="A2" s="118" t="s">
         <v>731</v>
       </c>
@@ -9464,7 +9510,7 @@
       <c r="F2" s="36"/>
       <c r="G2" s="42"/>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="28.5">
       <c r="A3" s="118" t="s">
         <v>732</v>
       </c>
@@ -9481,7 +9527,7 @@
       <c r="F3" s="36"/>
       <c r="G3" s="43"/>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="28.5">
       <c r="A4" s="118" t="s">
         <v>733</v>
       </c>
@@ -9498,7 +9544,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="43"/>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="28.5">
       <c r="A5" s="118" t="s">
         <v>1016</v>
       </c>
@@ -9519,7 +9565,7 @@
       </c>
       <c r="G5" s="100"/>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="28.5">
       <c r="A6" s="118" t="s">
         <v>1017</v>
       </c>
@@ -9557,17 +9603,17 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="109" t="s">
         <v>53</v>
       </c>
@@ -9805,20 +9851,20 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="113" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="83" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.875" style="113" customWidth="1"/>
+    <col min="2" max="2" width="18.875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="27.75" style="83" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="82" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="82" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" style="113" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="113" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.5703125" style="113" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="113"/>
+    <col min="5" max="5" width="13.25" style="82" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.125" style="113" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="113" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.625" style="113" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="113"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="93" t="s">
         <v>53</v>
       </c>
@@ -9844,7 +9890,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45">
+    <row r="2" spans="1:11" ht="42.75">
       <c r="A2" s="92" t="s">
         <v>669</v>
       </c>
@@ -9866,7 +9912,7 @@
       <c r="G2" s="103"/>
       <c r="H2" s="103"/>
     </row>
-    <row r="3" spans="1:11" ht="45">
+    <row r="3" spans="1:11" ht="42.75">
       <c r="A3" s="92" t="s">
         <v>672</v>
       </c>
@@ -9909,23 +9955,23 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="81" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="83" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.875" style="81" customWidth="1"/>
+    <col min="2" max="2" width="18.875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="27.75" style="83" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="82" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="82" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" style="81" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="81" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="81" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.5703125" style="81" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="81"/>
-    <col min="11" max="11" width="37.5703125" style="81" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="81"/>
+    <col min="5" max="5" width="13.25" style="82" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.125" style="81" customWidth="1"/>
+    <col min="7" max="7" width="16.625" style="81" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.875" style="81" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.625" style="81" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="81"/>
+    <col min="11" max="11" width="37.625" style="81" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="93" t="s">
         <v>53</v>
       </c>
@@ -9960,7 +10006,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30">
+    <row r="2" spans="1:11" ht="28.5">
       <c r="A2" s="92" t="s">
         <v>669</v>
       </c>
@@ -9985,7 +10031,7 @@
       </c>
       <c r="K2" s="90"/>
     </row>
-    <row r="3" spans="1:11" ht="30">
+    <row r="3" spans="1:11" ht="28.5">
       <c r="A3" s="92" t="s">
         <v>672</v>
       </c>
@@ -10006,7 +10052,7 @@
       <c r="J3" s="103"/>
       <c r="K3" s="103"/>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:11" ht="28.5">
       <c r="A4" s="92" t="s">
         <v>674</v>
       </c>
@@ -10031,7 +10077,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30">
+    <row r="5" spans="1:11" ht="28.5">
       <c r="A5" s="92" t="s">
         <v>675</v>
       </c>
@@ -10056,7 +10102,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45">
+    <row r="6" spans="1:11" ht="42.75">
       <c r="A6" s="92" t="s">
         <v>676</v>
       </c>
@@ -10081,7 +10127,7 @@
       </c>
       <c r="K6" s="90"/>
     </row>
-    <row r="7" spans="1:11" ht="45">
+    <row r="7" spans="1:11" ht="42.75">
       <c r="A7" s="92" t="s">
         <v>677</v>
       </c>
@@ -10106,7 +10152,7 @@
       </c>
       <c r="K7" s="90"/>
     </row>
-    <row r="8" spans="1:11" ht="45">
+    <row r="8" spans="1:11" ht="42.75">
       <c r="A8" s="92" t="s">
         <v>679</v>
       </c>
@@ -10135,7 +10181,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45">
+    <row r="9" spans="1:11" ht="42.75">
       <c r="A9" s="92" t="s">
         <v>680</v>
       </c>
@@ -10164,7 +10210,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30">
+    <row r="10" spans="1:11" ht="28.5">
       <c r="A10" s="92" t="s">
         <v>682</v>
       </c>
@@ -10189,7 +10235,7 @@
       </c>
       <c r="K10" s="90"/>
     </row>
-    <row r="11" spans="1:11" ht="30">
+    <row r="11" spans="1:11" ht="28.5">
       <c r="A11" s="92" t="s">
         <v>684</v>
       </c>
@@ -10216,7 +10262,7 @@
       </c>
       <c r="K11" s="90"/>
     </row>
-    <row r="12" spans="1:11" ht="30">
+    <row r="12" spans="1:11" ht="28.5">
       <c r="A12" s="92" t="s">
         <v>686</v>
       </c>
@@ -10239,7 +10285,7 @@
       <c r="J12" s="103"/>
       <c r="K12" s="103"/>
     </row>
-    <row r="13" spans="1:11" ht="45">
+    <row r="13" spans="1:11" ht="42.75">
       <c r="A13" s="92" t="s">
         <v>687</v>
       </c>
@@ -10266,7 +10312,7 @@
       </c>
       <c r="K13" s="90"/>
     </row>
-    <row r="14" spans="1:11" ht="45">
+    <row r="14" spans="1:11" ht="42.75">
       <c r="A14" s="92" t="s">
         <v>688</v>
       </c>
@@ -10293,7 +10339,7 @@
       </c>
       <c r="K14" s="103"/>
     </row>
-    <row r="15" spans="1:11" ht="60">
+    <row r="15" spans="1:11" ht="57">
       <c r="A15" s="92" t="s">
         <v>689</v>
       </c>
@@ -10324,7 +10370,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="60">
+    <row r="16" spans="1:11" ht="57">
       <c r="A16" s="92" t="s">
         <v>690</v>
       </c>
@@ -10355,7 +10401,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30">
+    <row r="17" spans="1:11" ht="28.5">
       <c r="A17" s="92" t="s">
         <v>692</v>
       </c>
@@ -10382,7 +10428,7 @@
       </c>
       <c r="K17" s="90"/>
     </row>
-    <row r="18" spans="1:11" ht="60">
+    <row r="18" spans="1:11" ht="57">
       <c r="A18" s="92" t="s">
         <v>693</v>
       </c>
@@ -10406,7 +10452,7 @@
       </c>
       <c r="K18" s="90"/>
     </row>
-    <row r="19" spans="1:11" ht="60">
+    <row r="19" spans="1:11" ht="57">
       <c r="A19" s="92" t="s">
         <v>710</v>
       </c>
@@ -10450,15 +10496,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="26"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.125" style="26"/>
+    <col min="3" max="3" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="26" customFormat="1">
+    <row r="1" spans="1:5" s="26" customFormat="1" ht="15">
       <c r="A1" s="30" t="s">
         <v>53</v>
       </c>
@@ -10492,7 +10538,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45">
+    <row r="3" spans="1:5" ht="42.75">
       <c r="A3" s="103" t="s">
         <v>735</v>
       </c>
@@ -10509,7 +10555,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="135">
+    <row r="4" spans="1:5" ht="128.25">
       <c r="A4" s="103" t="s">
         <v>736</v>
       </c>
@@ -10560,7 +10606,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="28.5">
       <c r="A7" s="103" t="s">
         <v>739</v>
       </c>
@@ -10594,12 +10640,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="9" style="82"/>
-    <col min="3" max="3" width="25.7109375" style="82" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="82" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="82" customWidth="1"/>
+    <col min="3" max="3" width="25.75" style="82" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" style="82" customWidth="1"/>
+    <col min="5" max="5" width="11.25" style="82" customWidth="1"/>
     <col min="6" max="16384" width="9" style="82"/>
   </cols>
   <sheetData>
@@ -10661,19 +10707,19 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="34" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.25" customWidth="1"/>
+    <col min="7" max="7" width="23.875" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="26.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="55" t="s">
         <v>53</v>
       </c>
@@ -10705,7 +10751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30">
+    <row r="2" spans="1:10" ht="28.5">
       <c r="A2" s="59" t="s">
         <v>632</v>
       </c>
@@ -10737,7 +10783,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30">
+    <row r="3" spans="1:10" ht="28.5">
       <c r="A3" s="61" t="s">
         <v>242</v>
       </c>
@@ -10761,7 +10807,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60">
+    <row r="4" spans="1:10" ht="57">
       <c r="A4" s="61" t="s">
         <v>243</v>
       </c>
@@ -10802,16 +10848,16 @@
       <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="26"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="1" max="2" width="9.125" style="26"/>
+    <col min="3" max="3" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.375" customWidth="1"/>
+    <col min="5" max="5" width="28.25" customWidth="1"/>
     <col min="6" max="6" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="26" customFormat="1">
+    <row r="1" spans="1:6" s="26" customFormat="1" ht="15">
       <c r="A1" s="20" t="s">
         <v>53</v>
       </c>
@@ -10964,16 +11010,16 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="81"/>
-    <col min="3" max="3" width="30.140625" style="81" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="81" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="81" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="81"/>
+    <col min="1" max="2" width="9.125" style="81"/>
+    <col min="3" max="3" width="30.125" style="81" customWidth="1"/>
+    <col min="4" max="4" width="31.125" style="81" customWidth="1"/>
+    <col min="5" max="5" width="31.25" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.125" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -11174,17 +11220,17 @@
       <selection activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="11.25" customWidth="1"/>
+    <col min="8" max="8" width="26.625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
@@ -11210,7 +11256,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
+    <row r="2" spans="1:8" ht="28.5">
       <c r="A2" s="21" t="s">
         <v>50</v>
       </c>
@@ -11236,7 +11282,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="28.5">
       <c r="A3" s="85" t="s">
         <v>74</v>
       </c>
@@ -11262,7 +11308,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:8" ht="28.5">
       <c r="A4" s="85" t="s">
         <v>82</v>
       </c>
@@ -11288,7 +11334,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="28.5">
       <c r="A5" s="85" t="s">
         <v>86</v>
       </c>
@@ -11314,7 +11360,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="28.5">
       <c r="A6" s="85" t="s">
         <v>87</v>
       </c>
@@ -11340,7 +11386,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30">
+    <row r="7" spans="1:8" ht="28.5">
       <c r="A7" s="85" t="s">
         <v>88</v>
       </c>
@@ -11366,7 +11412,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
+    <row r="8" spans="1:8" ht="28.5">
       <c r="A8" s="85" t="s">
         <v>89</v>
       </c>
@@ -11392,7 +11438,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30">
+    <row r="9" spans="1:8" ht="28.5">
       <c r="A9" s="85" t="s">
         <v>90</v>
       </c>
@@ -11418,7 +11464,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:8" ht="28.5">
       <c r="A10" s="85" t="s">
         <v>91</v>
       </c>
@@ -11444,7 +11490,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="28.5">
       <c r="A11" s="85" t="s">
         <v>92</v>
       </c>
@@ -11470,7 +11516,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="28.5">
       <c r="A12" s="85" t="s">
         <v>93</v>
       </c>
@@ -11496,7 +11542,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30">
+    <row r="13" spans="1:8" ht="28.5">
       <c r="A13" s="85" t="s">
         <v>94</v>
       </c>
@@ -11522,7 +11568,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="28.5">
       <c r="A14" s="85" t="s">
         <v>95</v>
       </c>
@@ -11548,7 +11594,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30">
+    <row r="15" spans="1:8" ht="28.5">
       <c r="A15" s="85" t="s">
         <v>96</v>
       </c>
@@ -11574,7 +11620,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30">
+    <row r="16" spans="1:8" ht="28.5">
       <c r="A16" s="85" t="s">
         <v>97</v>
       </c>
@@ -11600,7 +11646,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30">
+    <row r="17" spans="1:8" ht="28.5">
       <c r="A17" s="85" t="s">
         <v>98</v>
       </c>
@@ -11626,7 +11672,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30">
+    <row r="18" spans="1:8" ht="28.5">
       <c r="A18" s="85" t="s">
         <v>99</v>
       </c>
@@ -11652,7 +11698,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30">
+    <row r="19" spans="1:8" ht="28.5">
       <c r="A19" s="85" t="s">
         <v>100</v>
       </c>
@@ -11678,7 +11724,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30">
+    <row r="20" spans="1:8" ht="28.5">
       <c r="A20" s="85" t="s">
         <v>101</v>
       </c>
@@ -11704,7 +11750,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30">
+    <row r="21" spans="1:8" ht="28.5">
       <c r="A21" s="85" t="s">
         <v>102</v>
       </c>
@@ -11730,7 +11776,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30">
+    <row r="22" spans="1:8" ht="28.5">
       <c r="A22" s="85" t="s">
         <v>103</v>
       </c>
@@ -11756,7 +11802,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30">
+    <row r="23" spans="1:8" ht="28.5">
       <c r="A23" s="85" t="s">
         <v>104</v>
       </c>
@@ -11782,7 +11828,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30">
+    <row r="24" spans="1:8" ht="28.5">
       <c r="A24" s="85" t="s">
         <v>105</v>
       </c>
@@ -11808,7 +11854,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30">
+    <row r="25" spans="1:8" ht="28.5">
       <c r="A25" s="85" t="s">
         <v>106</v>
       </c>
@@ -11834,7 +11880,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30">
+    <row r="26" spans="1:8" ht="28.5">
       <c r="A26" s="85" t="s">
         <v>107</v>
       </c>
@@ -11860,7 +11906,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30">
+    <row r="27" spans="1:8" ht="28.5">
       <c r="A27" s="85" t="s">
         <v>591</v>
       </c>
@@ -11886,7 +11932,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30">
+    <row r="28" spans="1:8" ht="28.5">
       <c r="A28" s="85" t="s">
         <v>592</v>
       </c>
@@ -11912,7 +11958,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30">
+    <row r="29" spans="1:8" ht="28.5">
       <c r="A29" s="85" t="s">
         <v>593</v>
       </c>
@@ -11938,7 +11984,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30">
+    <row r="30" spans="1:8" ht="28.5">
       <c r="A30" s="85" t="s">
         <v>594</v>
       </c>
@@ -11964,7 +12010,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30">
+    <row r="31" spans="1:8" ht="28.5">
       <c r="A31" s="85" t="s">
         <v>595</v>
       </c>
@@ -11990,7 +12036,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30">
+    <row r="32" spans="1:8" ht="28.5">
       <c r="A32" s="85" t="s">
         <v>596</v>
       </c>
@@ -12016,7 +12062,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30">
+    <row r="33" spans="1:8" ht="28.5">
       <c r="A33" s="85" t="s">
         <v>597</v>
       </c>
@@ -12042,7 +12088,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30">
+    <row r="34" spans="1:8" ht="28.5">
       <c r="A34" s="85" t="s">
         <v>598</v>
       </c>
@@ -12068,7 +12114,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30">
+    <row r="35" spans="1:8" ht="28.5">
       <c r="A35" s="85" t="s">
         <v>599</v>
       </c>
@@ -12094,7 +12140,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30">
+    <row r="36" spans="1:8" ht="28.5">
       <c r="A36" s="85" t="s">
         <v>600</v>
       </c>
@@ -12120,7 +12166,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="30">
+    <row r="37" spans="1:8" ht="28.5">
       <c r="A37" s="85" t="s">
         <v>601</v>
       </c>
@@ -12146,7 +12192,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30">
+    <row r="38" spans="1:8" ht="28.5">
       <c r="A38" s="85" t="s">
         <v>602</v>
       </c>
@@ -12172,7 +12218,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="30">
+    <row r="39" spans="1:8" ht="28.5">
       <c r="A39" s="85" t="s">
         <v>603</v>
       </c>
@@ -12198,7 +12244,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="30">
+    <row r="40" spans="1:8" ht="28.5">
       <c r="A40" s="85" t="s">
         <v>111</v>
       </c>
@@ -12224,7 +12270,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="30">
+    <row r="41" spans="1:8" ht="28.5">
       <c r="A41" s="85" t="s">
         <v>112</v>
       </c>
@@ -12250,7 +12296,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30">
+    <row r="42" spans="1:8" ht="28.5">
       <c r="A42" s="85" t="s">
         <v>113</v>
       </c>
@@ -12276,7 +12322,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="30">
+    <row r="43" spans="1:8" ht="28.5">
       <c r="A43" s="85" t="s">
         <v>114</v>
       </c>
@@ -12302,7 +12348,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="30">
+    <row r="44" spans="1:8" ht="28.5">
       <c r="A44" s="85" t="s">
         <v>115</v>
       </c>
@@ -12328,7 +12374,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="30">
+    <row r="45" spans="1:8" ht="28.5">
       <c r="A45" s="85" t="s">
         <v>116</v>
       </c>
@@ -12354,7 +12400,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30">
+    <row r="46" spans="1:8" ht="28.5">
       <c r="A46" s="85" t="s">
         <v>117</v>
       </c>
@@ -12380,7 +12426,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="30">
+    <row r="47" spans="1:8" ht="28.5">
       <c r="A47" s="85" t="s">
         <v>118</v>
       </c>
@@ -12406,7 +12452,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30">
+    <row r="48" spans="1:8" ht="28.5">
       <c r="A48" s="85" t="s">
         <v>119</v>
       </c>
@@ -12432,7 +12478,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="30">
+    <row r="49" spans="1:8" ht="28.5">
       <c r="A49" s="85" t="s">
         <v>120</v>
       </c>
@@ -12458,7 +12504,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="30">
+    <row r="50" spans="1:8" ht="28.5">
       <c r="A50" s="85" t="s">
         <v>121</v>
       </c>
@@ -12484,7 +12530,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="30">
+    <row r="51" spans="1:8" ht="28.5">
       <c r="A51" s="85" t="s">
         <v>122</v>
       </c>
@@ -12510,7 +12556,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="30">
+    <row r="52" spans="1:8" ht="28.5">
       <c r="A52" s="85" t="s">
         <v>123</v>
       </c>
@@ -12536,7 +12582,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="30">
+    <row r="53" spans="1:8" ht="28.5">
       <c r="A53" s="85" t="s">
         <v>124</v>
       </c>
@@ -12562,7 +12608,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="30">
+    <row r="54" spans="1:8" ht="28.5">
       <c r="A54" s="85" t="s">
         <v>125</v>
       </c>
@@ -12588,7 +12634,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="30">
+    <row r="55" spans="1:8" ht="28.5">
       <c r="A55" s="85" t="s">
         <v>126</v>
       </c>
@@ -12614,7 +12660,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="30">
+    <row r="56" spans="1:8" ht="28.5">
       <c r="A56" s="85" t="s">
         <v>127</v>
       </c>
@@ -12640,7 +12686,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="30">
+    <row r="57" spans="1:8" ht="28.5">
       <c r="A57" s="85" t="s">
         <v>128</v>
       </c>
@@ -12666,7 +12712,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="30">
+    <row r="58" spans="1:8" ht="28.5">
       <c r="A58" s="85" t="s">
         <v>129</v>
       </c>
@@ -12692,7 +12738,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="30">
+    <row r="59" spans="1:8" ht="28.5">
       <c r="A59" s="85" t="s">
         <v>130</v>
       </c>
@@ -12718,7 +12764,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="30">
+    <row r="60" spans="1:8" ht="28.5">
       <c r="A60" s="85" t="s">
         <v>131</v>
       </c>
@@ -12744,7 +12790,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="30">
+    <row r="61" spans="1:8" ht="28.5">
       <c r="A61" s="85" t="s">
         <v>132</v>
       </c>
@@ -12770,7 +12816,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="30">
+    <row r="62" spans="1:8" ht="28.5">
       <c r="A62" s="85" t="s">
         <v>133</v>
       </c>
@@ -12796,7 +12842,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="30">
+    <row r="63" spans="1:8" ht="28.5">
       <c r="A63" s="85" t="s">
         <v>134</v>
       </c>
@@ -12822,7 +12868,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="30">
+    <row r="64" spans="1:8" ht="28.5">
       <c r="A64" s="85" t="s">
         <v>135</v>
       </c>
@@ -12848,7 +12894,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="30">
+    <row r="65" spans="1:8" ht="28.5">
       <c r="A65" s="85" t="s">
         <v>136</v>
       </c>
@@ -12874,7 +12920,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="30">
+    <row r="66" spans="1:8" ht="28.5">
       <c r="A66" s="85" t="s">
         <v>137</v>
       </c>
@@ -12900,7 +12946,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="30">
+    <row r="67" spans="1:8" ht="28.5">
       <c r="A67" s="85" t="s">
         <v>138</v>
       </c>
@@ -12926,7 +12972,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30">
+    <row r="68" spans="1:8" ht="28.5">
       <c r="A68" s="85" t="s">
         <v>139</v>
       </c>
@@ -12952,7 +12998,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30">
+    <row r="69" spans="1:8" ht="28.5">
       <c r="A69" s="85" t="s">
         <v>140</v>
       </c>
@@ -12978,7 +13024,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30">
+    <row r="70" spans="1:8" ht="28.5">
       <c r="A70" s="85" t="s">
         <v>141</v>
       </c>
@@ -13004,7 +13050,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="30">
+    <row r="71" spans="1:8" ht="28.5">
       <c r="A71" s="85" t="s">
         <v>142</v>
       </c>
@@ -13030,7 +13076,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="30">
+    <row r="72" spans="1:8">
       <c r="A72" s="85" t="s">
         <v>143</v>
       </c>
@@ -13056,7 +13102,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="30">
+    <row r="73" spans="1:8">
       <c r="A73" s="85" t="s">
         <v>144</v>
       </c>
@@ -13082,7 +13128,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="30">
+    <row r="74" spans="1:8">
       <c r="A74" s="85" t="s">
         <v>145</v>
       </c>
@@ -13108,7 +13154,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="30">
+    <row r="75" spans="1:8">
       <c r="A75" s="85" t="s">
         <v>146</v>
       </c>
@@ -13134,7 +13180,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="30">
+    <row r="76" spans="1:8">
       <c r="A76" s="85" t="s">
         <v>147</v>
       </c>
@@ -13160,7 +13206,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="30">
+    <row r="77" spans="1:8">
       <c r="A77" s="85" t="s">
         <v>148</v>
       </c>
@@ -13186,7 +13232,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="30">
+    <row r="78" spans="1:8">
       <c r="A78" s="85" t="s">
         <v>149</v>
       </c>
@@ -13212,7 +13258,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="30">
+    <row r="79" spans="1:8">
       <c r="A79" s="85" t="s">
         <v>337</v>
       </c>
@@ -13238,7 +13284,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="30">
+    <row r="80" spans="1:8">
       <c r="A80" s="85" t="s">
         <v>338</v>
       </c>
@@ -13264,7 +13310,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="30">
+    <row r="81" spans="1:8">
       <c r="A81" s="85" t="s">
         <v>339</v>
       </c>
@@ -13290,7 +13336,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="30">
+    <row r="82" spans="1:8">
       <c r="A82" s="85" t="s">
         <v>340</v>
       </c>
@@ -13316,7 +13362,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="30">
+    <row r="83" spans="1:8">
       <c r="A83" s="85" t="s">
         <v>341</v>
       </c>
@@ -13342,7 +13388,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="30">
+    <row r="84" spans="1:8">
       <c r="A84" s="85" t="s">
         <v>342</v>
       </c>
@@ -13368,7 +13414,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="30">
+    <row r="85" spans="1:8">
       <c r="A85" s="85" t="s">
         <v>343</v>
       </c>
@@ -13394,7 +13440,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="30">
+    <row r="86" spans="1:8">
       <c r="A86" s="85" t="s">
         <v>344</v>
       </c>
@@ -13420,7 +13466,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="30">
+    <row r="87" spans="1:8">
       <c r="A87" s="85" t="s">
         <v>345</v>
       </c>
@@ -13446,7 +13492,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="30">
+    <row r="88" spans="1:8">
       <c r="A88" s="85" t="s">
         <v>346</v>
       </c>
@@ -13472,7 +13518,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="30">
+    <row r="89" spans="1:8">
       <c r="A89" s="85" t="s">
         <v>347</v>
       </c>
@@ -13498,7 +13544,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="30">
+    <row r="90" spans="1:8">
       <c r="A90" s="85" t="s">
         <v>367</v>
       </c>
@@ -13524,7 +13570,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="30">
+    <row r="91" spans="1:8">
       <c r="A91" s="85" t="s">
         <v>425</v>
       </c>
@@ -13550,7 +13596,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="30">
+    <row r="92" spans="1:8">
       <c r="A92" s="85" t="s">
         <v>426</v>
       </c>
@@ -13576,7 +13622,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="30">
+    <row r="93" spans="1:8">
       <c r="A93" s="85" t="s">
         <v>427</v>
       </c>
@@ -13602,7 +13648,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="30">
+    <row r="94" spans="1:8">
       <c r="A94" s="85" t="s">
         <v>428</v>
       </c>
@@ -13628,7 +13674,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="30">
+    <row r="95" spans="1:8">
       <c r="A95" s="85" t="s">
         <v>429</v>
       </c>
@@ -13654,7 +13700,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="30">
+    <row r="96" spans="1:8">
       <c r="A96" s="85" t="s">
         <v>430</v>
       </c>
@@ -13680,7 +13726,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30">
+    <row r="97" spans="1:8">
       <c r="A97" s="85" t="s">
         <v>431</v>
       </c>
@@ -13706,7 +13752,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="30">
+    <row r="98" spans="1:8">
       <c r="A98" s="85" t="s">
         <v>432</v>
       </c>
@@ -13732,7 +13778,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="30">
+    <row r="99" spans="1:8">
       <c r="A99" s="85" t="s">
         <v>443</v>
       </c>
@@ -13758,7 +13804,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="30">
+    <row r="100" spans="1:8">
       <c r="A100" s="85" t="s">
         <v>444</v>
       </c>
@@ -13784,7 +13830,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="30">
+    <row r="101" spans="1:8">
       <c r="A101" s="85" t="s">
         <v>445</v>
       </c>
@@ -13810,7 +13856,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="30">
+    <row r="102" spans="1:8">
       <c r="A102" s="85" t="s">
         <v>446</v>
       </c>
@@ -13836,7 +13882,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="30">
+    <row r="103" spans="1:8">
       <c r="A103" s="85" t="s">
         <v>447</v>
       </c>
@@ -13862,7 +13908,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="30">
+    <row r="104" spans="1:8">
       <c r="A104" s="85" t="s">
         <v>448</v>
       </c>
@@ -13888,7 +13934,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="30">
+    <row r="105" spans="1:8">
       <c r="A105" s="85" t="s">
         <v>449</v>
       </c>
@@ -13914,7 +13960,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="30">
+    <row r="106" spans="1:8">
       <c r="A106" s="85" t="s">
         <v>450</v>
       </c>
@@ -13940,7 +13986,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="30">
+    <row r="107" spans="1:8">
       <c r="A107" s="85" t="s">
         <v>451</v>
       </c>
@@ -13966,7 +14012,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="30">
+    <row r="108" spans="1:8">
       <c r="A108" s="85" t="s">
         <v>452</v>
       </c>
@@ -13992,7 +14038,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="30">
+    <row r="109" spans="1:8">
       <c r="A109" s="85" t="s">
         <v>453</v>
       </c>
@@ -14018,7 +14064,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="30">
+    <row r="110" spans="1:8">
       <c r="A110" s="85" t="s">
         <v>454</v>
       </c>
@@ -14044,7 +14090,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="30">
+    <row r="111" spans="1:8">
       <c r="A111" s="85" t="s">
         <v>455</v>
       </c>
@@ -14070,7 +14116,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="30">
+    <row r="112" spans="1:8">
       <c r="A112" s="85" t="s">
         <v>456</v>
       </c>
@@ -14096,7 +14142,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="30">
+    <row r="113" spans="1:8">
       <c r="A113" s="85" t="s">
         <v>457</v>
       </c>
@@ -14122,7 +14168,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="30">
+    <row r="114" spans="1:8">
       <c r="A114" s="85" t="s">
         <v>458</v>
       </c>
@@ -14148,7 +14194,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="30">
+    <row r="115" spans="1:8">
       <c r="A115" s="85" t="s">
         <v>459</v>
       </c>
@@ -14174,7 +14220,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="30">
+    <row r="116" spans="1:8">
       <c r="A116" s="85" t="s">
         <v>604</v>
       </c>
@@ -14200,7 +14246,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="30">
+    <row r="117" spans="1:8">
       <c r="A117" s="85" t="s">
         <v>605</v>
       </c>
@@ -14226,7 +14272,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="30">
+    <row r="118" spans="1:8">
       <c r="A118" s="85" t="s">
         <v>606</v>
       </c>
@@ -14252,7 +14298,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="30">
+    <row r="119" spans="1:8">
       <c r="A119" s="85" t="s">
         <v>607</v>
       </c>
@@ -14278,7 +14324,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="30">
+    <row r="120" spans="1:8">
       <c r="A120" s="85" t="s">
         <v>608</v>
       </c>
@@ -14304,7 +14350,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="30">
+    <row r="121" spans="1:8">
       <c r="A121" s="85" t="s">
         <v>609</v>
       </c>
@@ -14330,7 +14376,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="30">
+    <row r="122" spans="1:8">
       <c r="A122" s="85" t="s">
         <v>610</v>
       </c>
@@ -14356,7 +14402,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="30">
+    <row r="123" spans="1:8">
       <c r="A123" s="85" t="s">
         <v>611</v>
       </c>
@@ -14382,7 +14428,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="30">
+    <row r="124" spans="1:8">
       <c r="A124" s="85" t="s">
         <v>612</v>
       </c>
@@ -14408,7 +14454,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="30">
+    <row r="125" spans="1:8">
       <c r="A125" s="85" t="s">
         <v>613</v>
       </c>
@@ -14434,7 +14480,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="30">
+    <row r="126" spans="1:8">
       <c r="A126" s="85" t="s">
         <v>614</v>
       </c>
@@ -14460,7 +14506,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="30">
+    <row r="127" spans="1:8">
       <c r="A127" s="85" t="s">
         <v>615</v>
       </c>
@@ -14486,7 +14532,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="30">
+    <row r="128" spans="1:8">
       <c r="A128" s="85" t="s">
         <v>616</v>
       </c>
@@ -14512,7 +14558,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="30">
+    <row r="129" spans="1:8">
       <c r="A129" s="85" t="s">
         <v>617</v>
       </c>
@@ -14538,7 +14584,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="30">
+    <row r="130" spans="1:8">
       <c r="A130" s="85" t="s">
         <v>618</v>
       </c>
@@ -14564,7 +14610,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="30">
+    <row r="131" spans="1:8">
       <c r="A131" s="85" t="s">
         <v>619</v>
       </c>
@@ -14590,7 +14636,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="30">
+    <row r="132" spans="1:8" ht="28.5">
       <c r="A132" s="85" t="s">
         <v>620</v>
       </c>
@@ -14616,7 +14662,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="30">
+    <row r="133" spans="1:8" ht="28.5">
       <c r="A133" s="85" t="s">
         <v>621</v>
       </c>
@@ -14642,7 +14688,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="30">
+    <row r="134" spans="1:8" ht="28.5">
       <c r="A134" s="85" t="s">
         <v>622</v>
       </c>
@@ -14668,7 +14714,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="30">
+    <row r="135" spans="1:8" ht="28.5">
       <c r="A135" s="85" t="s">
         <v>623</v>
       </c>
@@ -14694,7 +14740,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="30">
+    <row r="136" spans="1:8" ht="28.5">
       <c r="A136" s="85" t="s">
         <v>624</v>
       </c>
@@ -14720,7 +14766,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="30">
+    <row r="137" spans="1:8" ht="28.5">
       <c r="A137" s="85" t="s">
         <v>660</v>
       </c>
@@ -14746,7 +14792,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="30">
+    <row r="138" spans="1:8" ht="28.5">
       <c r="A138" s="85" t="s">
         <v>661</v>
       </c>
@@ -14772,7 +14818,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="30">
+    <row r="139" spans="1:8" ht="28.5">
       <c r="A139" s="85" t="s">
         <v>662</v>
       </c>
@@ -14798,7 +14844,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="30">
+    <row r="140" spans="1:8" ht="28.5">
       <c r="A140" s="85" t="s">
         <v>663</v>
       </c>
@@ -14824,7 +14870,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="30">
+    <row r="141" spans="1:8" ht="28.5">
       <c r="A141" s="85" t="s">
         <v>664</v>
       </c>
@@ -14850,7 +14896,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="30">
+    <row r="142" spans="1:8" ht="28.5">
       <c r="A142" s="85" t="s">
         <v>846</v>
       </c>
@@ -14876,7 +14922,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="30">
+    <row r="143" spans="1:8" ht="28.5">
       <c r="A143" s="85" t="s">
         <v>976</v>
       </c>
@@ -14935,24 +14981,24 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="113"/>
-    <col min="2" max="2" width="10.28515625" style="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="113" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" style="70" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.7109375" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.140625" style="113"/>
-    <col min="8" max="8" width="18.7109375" style="113" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="113" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="61.28515625" style="113" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="113"/>
+    <col min="1" max="1" width="9.125" style="113"/>
+    <col min="2" max="2" width="10.25" style="113" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="113" customWidth="1"/>
+    <col min="4" max="4" width="36.75" style="70" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.375" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.75" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.125" style="113"/>
+    <col min="8" max="8" width="18.75" style="113" customWidth="1"/>
+    <col min="9" max="9" width="18.25" style="113" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="61.25" style="113" customWidth="1"/>
+    <col min="11" max="12" width="9.125" style="113"/>
     <col min="13" max="13" width="16" style="113" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="113"/>
+    <col min="14" max="16384" width="9.125" style="113"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="15">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -14993,7 +15039,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="165">
+    <row r="2" spans="1:13" ht="156.75">
       <c r="A2" s="85" t="s">
         <v>2</v>
       </c>
@@ -15030,7 +15076,7 @@
       </c>
       <c r="M2" s="79"/>
     </row>
-    <row r="3" spans="1:13" ht="135">
+    <row r="3" spans="1:13" ht="128.25">
       <c r="A3" s="85" t="s">
         <v>8</v>
       </c>
@@ -15063,7 +15109,7 @@
       <c r="L3" s="79"/>
       <c r="M3" s="79"/>
     </row>
-    <row r="4" spans="1:13" ht="120">
+    <row r="4" spans="1:13" ht="114">
       <c r="A4" s="85" t="s">
         <v>44</v>
       </c>
@@ -15092,7 +15138,7 @@
       <c r="L4" s="79"/>
       <c r="M4" s="79"/>
     </row>
-    <row r="5" spans="1:13" ht="105">
+    <row r="5" spans="1:13" ht="85.5">
       <c r="A5" s="85" t="s">
         <v>84</v>
       </c>
@@ -15123,7 +15169,7 @@
       <c r="L5" s="79"/>
       <c r="M5" s="79"/>
     </row>
-    <row r="6" spans="1:13" ht="135">
+    <row r="6" spans="1:13" ht="128.25">
       <c r="A6" s="85" t="s">
         <v>175</v>
       </c>
@@ -15158,7 +15204,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="135">
+    <row r="7" spans="1:13" ht="128.25">
       <c r="A7" s="85" t="s">
         <v>204</v>
       </c>
@@ -15193,7 +15239,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="195">
+    <row r="8" spans="1:13" ht="171">
       <c r="A8" s="85" t="s">
         <v>353</v>
       </c>
@@ -15232,7 +15278,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="150">
+    <row r="9" spans="1:13" ht="142.5">
       <c r="A9" s="85" t="s">
         <v>44</v>
       </c>
@@ -15261,17 +15307,17 @@
       <c r="L9" s="79"/>
       <c r="M9" s="79"/>
     </row>
-    <row r="10" spans="1:13" ht="330">
+    <row r="10" spans="1:13" ht="300">
       <c r="A10" s="124" t="s">
         <v>956</v>
       </c>
       <c r="B10" s="125" t="s">
         <v>959</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="141" t="s">
         <v>958</v>
       </c>
-      <c r="D10" s="144" t="s">
+      <c r="D10" s="142" t="s">
         <v>955</v>
       </c>
       <c r="E10" s="100"/>
@@ -15290,7 +15336,7 @@
       <c r="L10" s="100"/>
       <c r="M10" s="100"/>
     </row>
-    <row r="11" spans="1:13" ht="60">
+    <row r="11" spans="1:13" ht="42.75">
       <c r="A11" s="124" t="s">
         <v>972</v>
       </c>
@@ -15300,7 +15346,7 @@
       <c r="C11" s="86" t="s">
         <v>981</v>
       </c>
-      <c r="D11" s="144" t="s">
+      <c r="D11" s="142" t="s">
         <v>973</v>
       </c>
       <c r="E11" s="100" t="s">
@@ -15324,10 +15370,10 @@
         <v>1015</v>
       </c>
       <c r="B12" s="125" t="s">
-        <v>1067</v>
+        <v>1062</v>
       </c>
       <c r="C12" s="86" t="s">
-        <v>1063</v>
+        <v>1058</v>
       </c>
       <c r="D12" s="128" t="s">
         <v>1022</v>
@@ -15342,24 +15388,24 @@
         <v>75</v>
       </c>
       <c r="J12" s="128" t="s">
-        <v>1064</v>
+        <v>1059</v>
       </c>
       <c r="K12" s="100"/>
       <c r="L12" s="100"/>
       <c r="M12" s="100"/>
     </row>
-    <row r="13" spans="1:13" ht="75">
+    <row r="13" spans="1:13" ht="57">
       <c r="A13" s="124" t="s">
         <v>1023</v>
       </c>
       <c r="B13" s="100" t="s">
-        <v>1067</v>
+        <v>1062</v>
       </c>
       <c r="C13" s="100" t="s">
-        <v>1066</v>
+        <v>1061</v>
       </c>
       <c r="D13" s="128" t="s">
-        <v>1068</v>
+        <v>1063</v>
       </c>
       <c r="E13" s="100"/>
       <c r="F13" s="100"/>
@@ -15371,7 +15417,7 @@
         <v>75</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
       <c r="K13" s="100"/>
       <c r="L13" s="100"/>
@@ -15399,15 +15445,15 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
@@ -15547,19 +15593,19 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1" collapsed="1"/>
     <col min="3" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="30">
       <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
@@ -15588,7 +15634,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="54" t="s">
         <v>28</v>
       </c>
@@ -15617,7 +15663,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="54" t="s">
         <v>29</v>
       </c>
@@ -15646,7 +15692,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="54" t="s">
         <v>42</v>
       </c>
@@ -15675,7 +15721,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="54" t="s">
         <v>158</v>
       </c>
@@ -15704,7 +15750,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="54" t="s">
         <v>436</v>
       </c>
@@ -15733,7 +15779,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="54" t="s">
         <v>634</v>
       </c>
@@ -15762,7 +15808,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="54" t="s">
         <v>635</v>
       </c>
@@ -15791,7 +15837,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="54" t="s">
         <v>636</v>
       </c>
@@ -15837,16 +15883,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="30">
       <c r="A1" s="20" t="s">
         <v>53</v>
       </c>
@@ -15863,7 +15909,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="29" t="s">
         <v>283</v>
       </c>
@@ -15880,7 +15926,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="28.5">
       <c r="A3" s="29" t="s">
         <v>284</v>
       </c>
@@ -15912,16 +15958,16 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="30">
       <c r="A1" s="20" t="s">
         <v>53</v>
       </c>
@@ -15938,7 +15984,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="29" t="s">
         <v>283</v>
       </c>
@@ -15955,7 +16001,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="28.5">
       <c r="A3" s="29" t="s">
         <v>284</v>
       </c>
@@ -15972,7 +16018,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:5" ht="28.5">
       <c r="A4" s="29" t="s">
         <v>285</v>
       </c>
@@ -15989,7 +16035,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="28.5">
       <c r="A5" s="29" t="s">
         <v>286</v>
       </c>
@@ -16004,7 +16050,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="28.5">
       <c r="A6" s="29" t="s">
         <v>297</v>
       </c>
@@ -16019,7 +16065,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="28.5">
       <c r="A7" s="29" t="s">
         <v>298</v>
       </c>
@@ -16051,16 +16097,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="113" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.875" customWidth="1"/>
+    <col min="6" max="6" width="45.25" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30">
@@ -16098,7 +16144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60">
+    <row r="2" spans="1:11" ht="57">
       <c r="A2" s="38" t="s">
         <v>986</v>
       </c>
@@ -16131,7 +16177,7 @@
       </c>
       <c r="K2" s="53"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" s="38" t="s">
         <v>987</v>
       </c>
@@ -16146,7 +16192,7 @@
       <c r="J3" s="114"/>
       <c r="K3" s="114"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" s="38" t="s">
         <v>988</v>
       </c>
@@ -16178,18 +16224,18 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="113" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="113" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" style="113" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="113"/>
-    <col min="6" max="6" width="19.5703125" style="113" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="113"/>
+    <col min="1" max="1" width="6.625" style="113" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" style="113" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.25" style="113" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.375" style="113" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="113"/>
+    <col min="6" max="6" width="19.625" style="113" customWidth="1"/>
+    <col min="7" max="16384" width="9.125" style="113"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="30">
       <c r="A1" s="20" t="s">
         <v>53</v>
       </c>
@@ -16245,7 +16291,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="103" t="s">
         <v>993</v>
       </c>
@@ -16381,7 +16427,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="103" t="s">
         <v>1013</v>
       </c>
@@ -16434,18 +16480,18 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.25" customWidth="1"/>
+    <col min="5" max="5" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="20" t="s">
         <v>53</v>
       </c>
@@ -16468,7 +16514,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120">
+    <row r="2" spans="1:7" ht="114">
       <c r="A2" s="29" t="s">
         <v>283</v>
       </c>
@@ -16487,7 +16533,7 @@
       <c r="F2" s="36"/>
       <c r="G2" s="42"/>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="42.75">
       <c r="A3" s="29" t="s">
         <v>284</v>
       </c>
@@ -16504,7 +16550,7 @@
       <c r="F3" s="36"/>
       <c r="G3" s="43"/>
     </row>
-    <row r="4" spans="1:7" ht="120">
+    <row r="4" spans="1:7" ht="114">
       <c r="A4" s="29" t="s">
         <v>285</v>
       </c>
@@ -16523,7 +16569,7 @@
       </c>
       <c r="G4" s="42"/>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="42.75">
       <c r="A5" s="29" t="s">
         <v>286</v>
       </c>
@@ -16556,19 +16602,19 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="142" t="s">
+    <row r="1" spans="1:2" ht="15">
+      <c r="A1" s="140" t="s">
         <v>726</v>
       </c>
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="140" t="s">
         <v>36</v>
       </c>
     </row>
@@ -16590,7 +16636,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="100" t="s">
-        <v>1061</v>
+        <v>1056</v>
       </c>
       <c r="B4" s="102" t="s">
         <v>35</v>
@@ -16604,7 +16650,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="114" t="s">
-        <v>1062</v>
+        <v>1057</v>
       </c>
       <c r="B6" s="114"/>
     </row>
@@ -16618,19 +16664,19 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="95" t="s">
         <v>720</v>
       </c>
@@ -16683,6 +16729,78 @@
         <v>725</v>
       </c>
       <c r="B7" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="113" customFormat="1">
+      <c r="A8" s="100" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B8" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="113" customFormat="1">
+      <c r="A9" s="100" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B9" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="113" customFormat="1">
+      <c r="A10" s="100" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B10" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="113" customFormat="1">
+      <c r="A11" s="100" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B11" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="113" customFormat="1">
+      <c r="A12" s="100" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B12" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="113" customFormat="1">
+      <c r="A13" s="100" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B13" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="113" customFormat="1">
+      <c r="A14" s="100" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B14" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="113" customFormat="1">
+      <c r="A15" s="100" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B15" s="97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="114" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B16" s="97" t="s">
         <v>35</v>
       </c>
     </row>
@@ -16702,17 +16820,17 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -18393,17 +18511,17 @@
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -20006,17 +20124,17 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="15">
       <c r="A1" s="28" t="s">
         <v>53</v>
       </c>
@@ -21697,20 +21815,20 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15">
       <c r="A1" s="15" t="s">
         <v>53</v>
       </c>
@@ -21745,7 +21863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A2" s="14" t="s">
         <v>205</v>
       </c>
@@ -21778,7 +21896,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A3" s="84" t="s">
         <v>206</v>
       </c>
@@ -21811,7 +21929,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A4" s="84" t="s">
         <v>207</v>
       </c>
@@ -21844,7 +21962,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A5" s="84" t="s">
         <v>208</v>
       </c>
@@ -21877,7 +21995,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="75">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="71.25">
       <c r="A6" s="84" t="s">
         <v>209</v>
       </c>
@@ -21910,7 +22028,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A7" s="84" t="s">
         <v>210</v>
       </c>
@@ -21943,7 +22061,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A8" s="84" t="s">
         <v>211</v>
       </c>
@@ -21976,7 +22094,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A9" s="84" t="s">
         <v>212</v>
       </c>
@@ -22009,7 +22127,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A10" s="84" t="s">
         <v>213</v>
       </c>
@@ -22042,7 +22160,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="57">
       <c r="A11" s="84" t="s">
         <v>214</v>
       </c>
@@ -22075,7 +22193,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60">
+    <row r="12" spans="1:11" ht="57">
       <c r="A12" s="84" t="s">
         <v>215</v>
       </c>
@@ -22108,7 +22226,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60">
+    <row r="13" spans="1:11" ht="57">
       <c r="A13" s="84" t="s">
         <v>216</v>
       </c>
@@ -22141,7 +22259,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="60">
+    <row r="14" spans="1:11" ht="42.75">
       <c r="A14" s="84" t="s">
         <v>217</v>
       </c>
@@ -22172,7 +22290,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="23"/>
     </row>
-    <row r="15" spans="1:11" ht="60">
+    <row r="15" spans="1:11" ht="57">
       <c r="A15" s="84" t="s">
         <v>218</v>
       </c>
@@ -22203,7 +22321,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="23"/>
     </row>
-    <row r="16" spans="1:11" ht="60">
+    <row r="16" spans="1:11" ht="57">
       <c r="A16" s="84" t="s">
         <v>219</v>
       </c>
@@ -22234,7 +22352,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:11" s="81" customFormat="1" ht="60">
+    <row r="17" spans="1:11" s="81" customFormat="1" ht="57">
       <c r="A17" s="84" t="s">
         <v>220</v>
       </c>
@@ -22265,7 +22383,7 @@
       <c r="J17" s="79"/>
       <c r="K17" s="75"/>
     </row>
-    <row r="18" spans="1:11" s="81" customFormat="1" ht="60">
+    <row r="18" spans="1:11" s="81" customFormat="1" ht="57">
       <c r="A18" s="84" t="s">
         <v>221</v>
       </c>
@@ -22296,7 +22414,7 @@
       <c r="J18" s="79"/>
       <c r="K18" s="75"/>
     </row>
-    <row r="19" spans="1:11" ht="60">
+    <row r="19" spans="1:11" ht="57">
       <c r="A19" s="84" t="s">
         <v>222</v>
       </c>
@@ -22327,7 +22445,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="23"/>
     </row>
-    <row r="20" spans="1:11" ht="45">
+    <row r="20" spans="1:11" ht="42.75">
       <c r="A20" s="84" t="s">
         <v>223</v>
       </c>
@@ -22358,7 +22476,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="23"/>
     </row>
-    <row r="21" spans="1:11" ht="60">
+    <row r="21" spans="1:11" ht="57">
       <c r="A21" s="84" t="s">
         <v>224</v>
       </c>
@@ -22389,7 +22507,7 @@
       <c r="J21" s="19"/>
       <c r="K21" s="23"/>
     </row>
-    <row r="22" spans="1:11" ht="60">
+    <row r="22" spans="1:11" ht="57">
       <c r="A22" s="84" t="s">
         <v>225</v>
       </c>
@@ -22422,7 +22540,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="60">
+    <row r="23" spans="1:11" ht="57">
       <c r="A23" s="84" t="s">
         <v>226</v>
       </c>
@@ -22455,7 +22573,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="60">
+    <row r="24" spans="1:11" ht="57">
       <c r="A24" s="84" t="s">
         <v>227</v>
       </c>
@@ -22488,7 +22606,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="60">
+    <row r="25" spans="1:11" ht="57">
       <c r="A25" s="84" t="s">
         <v>228</v>
       </c>
@@ -22521,7 +22639,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="75">
+    <row r="26" spans="1:11" ht="71.25">
       <c r="A26" s="84" t="s">
         <v>229</v>
       </c>
@@ -22554,7 +22672,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="60">
+    <row r="27" spans="1:11" ht="57">
       <c r="A27" s="84" t="s">
         <v>230</v>
       </c>
@@ -22587,7 +22705,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60">
+    <row r="28" spans="1:11" ht="57">
       <c r="A28" s="84" t="s">
         <v>231</v>
       </c>
@@ -22620,7 +22738,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60">
+    <row r="29" spans="1:11" ht="57">
       <c r="A29" s="84" t="s">
         <v>232</v>
       </c>
@@ -22653,7 +22771,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60">
+    <row r="30" spans="1:11" ht="57">
       <c r="A30" s="84" t="s">
         <v>233</v>
       </c>
@@ -22686,7 +22804,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="60">
+    <row r="31" spans="1:11" ht="57">
       <c r="A31" s="84" t="s">
         <v>234</v>
       </c>
@@ -22719,7 +22837,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="60">
+    <row r="32" spans="1:11" ht="57">
       <c r="A32" s="84" t="s">
         <v>235</v>
       </c>
@@ -22752,7 +22870,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="60">
+    <row r="33" spans="1:11" ht="57">
       <c r="A33" s="84" t="s">
         <v>236</v>
       </c>
@@ -22785,7 +22903,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="60">
+    <row r="34" spans="1:11" ht="57">
       <c r="A34" s="84" t="s">
         <v>237</v>
       </c>
@@ -22816,7 +22934,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="23"/>
     </row>
-    <row r="35" spans="1:11" ht="60">
+    <row r="35" spans="1:11" ht="57">
       <c r="A35" s="84" t="s">
         <v>238</v>
       </c>
@@ -22847,7 +22965,7 @@
       <c r="J35" s="19"/>
       <c r="K35" s="23"/>
     </row>
-    <row r="36" spans="1:11" ht="60">
+    <row r="36" spans="1:11" ht="57">
       <c r="A36" s="84" t="s">
         <v>239</v>
       </c>
@@ -22878,7 +22996,7 @@
       <c r="J36" s="19"/>
       <c r="K36" s="23"/>
     </row>
-    <row r="37" spans="1:11" ht="60">
+    <row r="37" spans="1:11" ht="57">
       <c r="A37" s="84" t="s">
         <v>240</v>
       </c>
@@ -22909,7 +23027,7 @@
       <c r="J37" s="19"/>
       <c r="K37" s="23"/>
     </row>
-    <row r="38" spans="1:11" ht="60">
+    <row r="38" spans="1:11" ht="57">
       <c r="A38" s="84" t="s">
         <v>241</v>
       </c>
@@ -22940,7 +23058,7 @@
       <c r="J38" s="19"/>
       <c r="K38" s="23"/>
     </row>
-    <row r="39" spans="1:11" ht="60">
+    <row r="39" spans="1:11" ht="57">
       <c r="A39" s="84" t="s">
         <v>281</v>
       </c>
@@ -22971,7 +23089,7 @@
       <c r="J39" s="19"/>
       <c r="K39" s="23"/>
     </row>
-    <row r="40" spans="1:11" ht="45">
+    <row r="40" spans="1:11" ht="42.75">
       <c r="A40" s="84" t="s">
         <v>324</v>
       </c>
@@ -23002,7 +23120,7 @@
       <c r="J40" s="19"/>
       <c r="K40" s="23"/>
     </row>
-    <row r="41" spans="1:11" ht="60">
+    <row r="41" spans="1:11" ht="57">
       <c r="A41" s="84" t="s">
         <v>709</v>
       </c>
@@ -23033,7 +23151,7 @@
       <c r="J41" s="19"/>
       <c r="K41" s="23"/>
     </row>
-    <row r="42" spans="1:11" ht="60">
+    <row r="42" spans="1:11" ht="57">
       <c r="A42" s="84" t="s">
         <v>831</v>
       </c>
@@ -23066,7 +23184,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="75">
+    <row r="43" spans="1:11" ht="57">
       <c r="A43" s="84" t="s">
         <v>832</v>
       </c>
@@ -23099,7 +23217,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="75">
+    <row r="44" spans="1:11" ht="71.25">
       <c r="A44" s="84" t="s">
         <v>848</v>
       </c>
@@ -23132,7 +23250,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="75">
+    <row r="45" spans="1:11" ht="71.25">
       <c r="A45" s="84" t="s">
         <v>832</v>
       </c>
@@ -23163,7 +23281,7 @@
       <c r="J45" s="76"/>
       <c r="K45" s="114"/>
     </row>
-    <row r="46" spans="1:11" ht="75">
+    <row r="46" spans="1:11" ht="71.25">
       <c r="A46" s="84" t="s">
         <v>848</v>
       </c>

</xml_diff>